<commit_message>
nmv 18 10 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 6.1 TO 6.6.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 6.1 TO 6.6.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1732904D-9A7F-4ED1-AF8F-049A95A3D824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504E3982-D800-4F18-996B-D3D54E95A974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="6.1" sheetId="15" r:id="rId1"/>
-    <sheet name="total 6.1 to 6.6" sheetId="7" r:id="rId2"/>
+    <sheet name="6.2" sheetId="16" r:id="rId2"/>
+    <sheet name="total 6.1 to 6.6" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="190">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -1621,6 +1622,186 @@
   </si>
   <si>
     <t>76</t>
+  </si>
+  <si>
+    <t>6.2.1.1 :</t>
+  </si>
+  <si>
+    <t>6.2.1.2 :</t>
+  </si>
+  <si>
+    <t>6.2.1.3 :</t>
+  </si>
+  <si>
+    <t>6.2.1.4 :</t>
+  </si>
+  <si>
+    <t>6.2.1.5 :</t>
+  </si>
+  <si>
+    <t>6.2.1.6 :</t>
+  </si>
+  <si>
+    <t>6.2.1.7 :</t>
+  </si>
+  <si>
+    <t>6.2.2.1 :</t>
+  </si>
+  <si>
+    <t>6.2.2.2 :</t>
+  </si>
+  <si>
+    <t>6.2.2.3 :</t>
+  </si>
+  <si>
+    <t>6.2.2.4 :</t>
+  </si>
+  <si>
+    <t>6.2.2.5 :</t>
+  </si>
+  <si>
+    <t>6.2.2.6 :</t>
+  </si>
+  <si>
+    <t>6.2.2.7 :</t>
+  </si>
+  <si>
+    <t>6.2.3.1 :</t>
+  </si>
+  <si>
+    <t>6.2.3.2 :</t>
+  </si>
+  <si>
+    <t>6.2.3.3 :</t>
+  </si>
+  <si>
+    <t>6.2.3.4 :</t>
+  </si>
+  <si>
+    <t>6.2.3.5 :</t>
+  </si>
+  <si>
+    <t>6.2.4.1 :</t>
+  </si>
+  <si>
+    <t>6.2.4.2 :</t>
+  </si>
+  <si>
+    <t>6.2.4.3 :</t>
+  </si>
+  <si>
+    <t>6.2.4.4 :</t>
+  </si>
+  <si>
+    <t>6.2.4.5 :</t>
+  </si>
+  <si>
+    <t>6.2.5.1 :</t>
+  </si>
+  <si>
+    <t>6.2.5.2 :</t>
+  </si>
+  <si>
+    <t>6.2.5.3 :</t>
+  </si>
+  <si>
+    <t>6.2.5.4 :</t>
+  </si>
+  <si>
+    <t>6.2.5.5 :</t>
+  </si>
+  <si>
+    <t>6.2.6.1 :</t>
+  </si>
+  <si>
+    <t>6.2.6.2 :</t>
+  </si>
+  <si>
+    <t>6.2.6.3 :</t>
+  </si>
+  <si>
+    <t>6.2.6.4 :</t>
+  </si>
+  <si>
+    <t>6.2.7.1 :</t>
+  </si>
+  <si>
+    <t>6.2.7.2 :</t>
+  </si>
+  <si>
+    <t>6.2.7.3 :</t>
+  </si>
+  <si>
+    <t>6.2.7.4 :</t>
+  </si>
+  <si>
+    <t>6.2.7.5 :</t>
+  </si>
+  <si>
+    <t>6.2.8.1 :</t>
+  </si>
+  <si>
+    <t>6.2.8.2 :</t>
+  </si>
+  <si>
+    <t>6.2.8.3 :</t>
+  </si>
+  <si>
+    <t>6.2.8.4 :</t>
+  </si>
+  <si>
+    <t>6.2.8.5 :</t>
+  </si>
+  <si>
+    <t>6.2.8.6 :</t>
+  </si>
+  <si>
+    <t>6.2.9.1 :</t>
+  </si>
+  <si>
+    <t>6.2.9.2 :</t>
+  </si>
+  <si>
+    <t>6.2.9.3 :</t>
+  </si>
+  <si>
+    <t>6.2.9.4 :</t>
+  </si>
+  <si>
+    <t>6.2.10.1 :</t>
+  </si>
+  <si>
+    <t>6.2.10.2 :</t>
+  </si>
+  <si>
+    <t>6.2.10.3 :</t>
+  </si>
+  <si>
+    <t>6.2.10.4 :</t>
+  </si>
+  <si>
+    <t>6.2.10.5 :</t>
+  </si>
+  <si>
+    <t>6.2.10.6 :</t>
+  </si>
+  <si>
+    <t>6.2.10.7 :</t>
+  </si>
+  <si>
+    <t>6.2.11.1 :</t>
+  </si>
+  <si>
+    <t>6.2.11.2 :</t>
+  </si>
+  <si>
+    <t>6.2.11.3 :</t>
+  </si>
+  <si>
+    <t>6.2.11.4 :</t>
+  </si>
+  <si>
+    <t>59</t>
   </si>
 </sst>
 </file>
@@ -1817,7 +1998,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1911,6 +2092,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2194,9 +2378,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O79" sqref="O79"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E79" sqref="E79:J88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5293,6 +5477,2460 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D38C19-8B03-4797-B383-C63371C35E12}">
+  <dimension ref="A1:L71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M65" sqref="M65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="33">
+        <v>9</v>
+      </c>
+      <c r="C2" s="33">
+        <v>0</v>
+      </c>
+      <c r="D2" s="33">
+        <v>1</v>
+      </c>
+      <c r="E2" s="33">
+        <v>0</v>
+      </c>
+      <c r="F2" s="33">
+        <v>0</v>
+      </c>
+      <c r="G2" s="33">
+        <v>2</v>
+      </c>
+      <c r="H2" s="33">
+        <v>0</v>
+      </c>
+      <c r="I2" s="33">
+        <v>0</v>
+      </c>
+      <c r="J2" s="33">
+        <v>40</v>
+      </c>
+      <c r="K2" s="33">
+        <v>50</v>
+      </c>
+      <c r="L2" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="33">
+        <v>6</v>
+      </c>
+      <c r="C3" s="33">
+        <v>0</v>
+      </c>
+      <c r="D3" s="33">
+        <v>0</v>
+      </c>
+      <c r="E3" s="33">
+        <v>0</v>
+      </c>
+      <c r="F3" s="33">
+        <v>0</v>
+      </c>
+      <c r="G3" s="33">
+        <v>0</v>
+      </c>
+      <c r="H3" s="33">
+        <v>0</v>
+      </c>
+      <c r="I3" s="33">
+        <v>0</v>
+      </c>
+      <c r="J3" s="33">
+        <v>44</v>
+      </c>
+      <c r="K3" s="33">
+        <v>50</v>
+      </c>
+      <c r="L3" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="33">
+        <v>5</v>
+      </c>
+      <c r="C4" s="33">
+        <v>0</v>
+      </c>
+      <c r="D4" s="33">
+        <v>0</v>
+      </c>
+      <c r="E4" s="33">
+        <v>0</v>
+      </c>
+      <c r="F4" s="33">
+        <v>0</v>
+      </c>
+      <c r="G4" s="33">
+        <v>2</v>
+      </c>
+      <c r="H4" s="33">
+        <v>0</v>
+      </c>
+      <c r="I4" s="33">
+        <v>0</v>
+      </c>
+      <c r="J4" s="33">
+        <v>45</v>
+      </c>
+      <c r="K4" s="33">
+        <v>50</v>
+      </c>
+      <c r="L4" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="33">
+        <v>14</v>
+      </c>
+      <c r="C5" s="33">
+        <v>0</v>
+      </c>
+      <c r="D5" s="33">
+        <v>0</v>
+      </c>
+      <c r="E5" s="33">
+        <v>0</v>
+      </c>
+      <c r="F5" s="33">
+        <v>0</v>
+      </c>
+      <c r="G5" s="33">
+        <v>0</v>
+      </c>
+      <c r="H5" s="33">
+        <v>0</v>
+      </c>
+      <c r="I5" s="33">
+        <v>0</v>
+      </c>
+      <c r="J5" s="33">
+        <v>36</v>
+      </c>
+      <c r="K5" s="33">
+        <v>50</v>
+      </c>
+      <c r="L5" s="33">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="33">
+        <v>12</v>
+      </c>
+      <c r="C6" s="33">
+        <v>0</v>
+      </c>
+      <c r="D6" s="33">
+        <v>4</v>
+      </c>
+      <c r="E6" s="33">
+        <v>0</v>
+      </c>
+      <c r="F6" s="33">
+        <v>0</v>
+      </c>
+      <c r="G6" s="33">
+        <v>1</v>
+      </c>
+      <c r="H6" s="33">
+        <v>0</v>
+      </c>
+      <c r="I6" s="33">
+        <v>0</v>
+      </c>
+      <c r="J6" s="33">
+        <v>34</v>
+      </c>
+      <c r="K6" s="33">
+        <v>50</v>
+      </c>
+      <c r="L6" s="33">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="33">
+        <v>11</v>
+      </c>
+      <c r="C7" s="33">
+        <v>0</v>
+      </c>
+      <c r="D7" s="33">
+        <v>2</v>
+      </c>
+      <c r="E7" s="33">
+        <v>0</v>
+      </c>
+      <c r="F7" s="33">
+        <v>0</v>
+      </c>
+      <c r="G7" s="33">
+        <v>6</v>
+      </c>
+      <c r="H7" s="33">
+        <v>0</v>
+      </c>
+      <c r="I7" s="33">
+        <v>0</v>
+      </c>
+      <c r="J7" s="33">
+        <v>37</v>
+      </c>
+      <c r="K7" s="33">
+        <v>50</v>
+      </c>
+      <c r="L7" s="33">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="33">
+        <v>3</v>
+      </c>
+      <c r="C8" s="33">
+        <v>0</v>
+      </c>
+      <c r="D8" s="33">
+        <v>1</v>
+      </c>
+      <c r="E8" s="33">
+        <v>0</v>
+      </c>
+      <c r="F8" s="33">
+        <v>1</v>
+      </c>
+      <c r="G8" s="33">
+        <v>0</v>
+      </c>
+      <c r="H8" s="33">
+        <v>0</v>
+      </c>
+      <c r="I8" s="33">
+        <v>0</v>
+      </c>
+      <c r="J8" s="33">
+        <v>36</v>
+      </c>
+      <c r="K8" s="33">
+        <v>41</v>
+      </c>
+      <c r="L8" s="33">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="33">
+        <v>8</v>
+      </c>
+      <c r="C9" s="33">
+        <v>0</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0</v>
+      </c>
+      <c r="E9" s="33">
+        <v>0</v>
+      </c>
+      <c r="F9" s="33">
+        <v>0</v>
+      </c>
+      <c r="G9" s="33">
+        <v>2</v>
+      </c>
+      <c r="H9" s="33">
+        <v>0</v>
+      </c>
+      <c r="I9" s="33">
+        <v>0</v>
+      </c>
+      <c r="J9" s="33">
+        <v>42</v>
+      </c>
+      <c r="K9" s="33">
+        <v>50</v>
+      </c>
+      <c r="L9" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="33">
+        <v>9</v>
+      </c>
+      <c r="C10" s="33">
+        <v>0</v>
+      </c>
+      <c r="D10" s="33">
+        <v>1</v>
+      </c>
+      <c r="E10" s="33">
+        <v>0</v>
+      </c>
+      <c r="F10" s="33">
+        <v>0</v>
+      </c>
+      <c r="G10" s="33">
+        <v>4</v>
+      </c>
+      <c r="H10" s="33">
+        <v>0</v>
+      </c>
+      <c r="I10" s="33">
+        <v>0</v>
+      </c>
+      <c r="J10" s="33">
+        <v>40</v>
+      </c>
+      <c r="K10" s="33">
+        <v>50</v>
+      </c>
+      <c r="L10" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="33">
+        <v>12</v>
+      </c>
+      <c r="C11" s="33">
+        <v>0</v>
+      </c>
+      <c r="D11" s="33">
+        <v>0</v>
+      </c>
+      <c r="E11" s="33">
+        <v>0</v>
+      </c>
+      <c r="F11" s="33">
+        <v>0</v>
+      </c>
+      <c r="G11" s="33">
+        <v>0</v>
+      </c>
+      <c r="H11" s="33">
+        <v>0</v>
+      </c>
+      <c r="I11" s="33">
+        <v>0</v>
+      </c>
+      <c r="J11" s="33">
+        <v>38</v>
+      </c>
+      <c r="K11" s="33">
+        <v>50</v>
+      </c>
+      <c r="L11" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" s="33">
+        <v>9</v>
+      </c>
+      <c r="C12" s="33">
+        <v>0</v>
+      </c>
+      <c r="D12" s="33">
+        <v>0</v>
+      </c>
+      <c r="E12" s="33">
+        <v>0</v>
+      </c>
+      <c r="F12" s="33">
+        <v>0</v>
+      </c>
+      <c r="G12" s="33">
+        <v>2</v>
+      </c>
+      <c r="H12" s="33">
+        <v>0</v>
+      </c>
+      <c r="I12" s="33">
+        <v>0</v>
+      </c>
+      <c r="J12" s="33">
+        <v>41</v>
+      </c>
+      <c r="K12" s="33">
+        <v>50</v>
+      </c>
+      <c r="L12" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" s="33">
+        <v>0</v>
+      </c>
+      <c r="C13" s="33">
+        <v>0</v>
+      </c>
+      <c r="D13" s="33">
+        <v>0</v>
+      </c>
+      <c r="E13" s="33">
+        <v>0</v>
+      </c>
+      <c r="F13" s="33">
+        <v>0</v>
+      </c>
+      <c r="G13" s="33">
+        <v>6</v>
+      </c>
+      <c r="H13" s="33">
+        <v>0</v>
+      </c>
+      <c r="I13" s="33">
+        <v>0</v>
+      </c>
+      <c r="J13" s="33">
+        <v>50</v>
+      </c>
+      <c r="K13" s="33">
+        <v>50</v>
+      </c>
+      <c r="L13" s="33">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="33">
+        <v>8</v>
+      </c>
+      <c r="C14" s="33">
+        <v>0</v>
+      </c>
+      <c r="D14" s="33">
+        <v>0</v>
+      </c>
+      <c r="E14" s="33">
+        <v>0</v>
+      </c>
+      <c r="F14" s="33">
+        <v>0</v>
+      </c>
+      <c r="G14" s="33">
+        <v>5</v>
+      </c>
+      <c r="H14" s="33">
+        <v>0</v>
+      </c>
+      <c r="I14" s="33">
+        <v>0</v>
+      </c>
+      <c r="J14" s="33">
+        <v>42</v>
+      </c>
+      <c r="K14" s="33">
+        <v>50</v>
+      </c>
+      <c r="L14" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="33">
+        <v>12</v>
+      </c>
+      <c r="C15" s="33">
+        <v>0</v>
+      </c>
+      <c r="D15" s="33">
+        <v>0</v>
+      </c>
+      <c r="E15" s="33">
+        <v>0</v>
+      </c>
+      <c r="F15" s="33">
+        <v>1</v>
+      </c>
+      <c r="G15" s="33">
+        <v>4</v>
+      </c>
+      <c r="H15" s="33">
+        <v>0</v>
+      </c>
+      <c r="I15" s="33">
+        <v>0</v>
+      </c>
+      <c r="J15" s="33">
+        <v>48</v>
+      </c>
+      <c r="K15" s="33">
+        <v>61</v>
+      </c>
+      <c r="L15" s="33">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16" s="33">
+        <v>3</v>
+      </c>
+      <c r="C16" s="33">
+        <v>0</v>
+      </c>
+      <c r="D16" s="33">
+        <v>0</v>
+      </c>
+      <c r="E16" s="33">
+        <v>0</v>
+      </c>
+      <c r="F16" s="33">
+        <v>0</v>
+      </c>
+      <c r="G16" s="33">
+        <v>1</v>
+      </c>
+      <c r="H16" s="33">
+        <v>0</v>
+      </c>
+      <c r="I16" s="33">
+        <v>0</v>
+      </c>
+      <c r="J16" s="33">
+        <v>47</v>
+      </c>
+      <c r="K16" s="33">
+        <v>50</v>
+      </c>
+      <c r="L16" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="B17" s="33">
+        <v>7</v>
+      </c>
+      <c r="C17" s="33">
+        <v>0</v>
+      </c>
+      <c r="D17" s="33">
+        <v>0</v>
+      </c>
+      <c r="E17" s="33">
+        <v>0</v>
+      </c>
+      <c r="F17" s="33">
+        <v>0</v>
+      </c>
+      <c r="G17" s="33">
+        <v>2</v>
+      </c>
+      <c r="H17" s="33">
+        <v>0</v>
+      </c>
+      <c r="I17" s="33">
+        <v>0</v>
+      </c>
+      <c r="J17" s="33">
+        <v>43</v>
+      </c>
+      <c r="K17" s="33">
+        <v>50</v>
+      </c>
+      <c r="L17" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="B18" s="33">
+        <v>12</v>
+      </c>
+      <c r="C18" s="33">
+        <v>0</v>
+      </c>
+      <c r="D18" s="33">
+        <v>0</v>
+      </c>
+      <c r="E18" s="33">
+        <v>0</v>
+      </c>
+      <c r="F18" s="33">
+        <v>0</v>
+      </c>
+      <c r="G18" s="33">
+        <v>3</v>
+      </c>
+      <c r="H18" s="33">
+        <v>0</v>
+      </c>
+      <c r="I18" s="33">
+        <v>0</v>
+      </c>
+      <c r="J18" s="33">
+        <v>38</v>
+      </c>
+      <c r="K18" s="33">
+        <v>50</v>
+      </c>
+      <c r="L18" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="B19" s="33">
+        <v>8</v>
+      </c>
+      <c r="C19" s="33">
+        <v>0</v>
+      </c>
+      <c r="D19" s="33">
+        <v>0</v>
+      </c>
+      <c r="E19" s="33">
+        <v>0</v>
+      </c>
+      <c r="F19" s="33">
+        <v>0</v>
+      </c>
+      <c r="G19" s="33">
+        <v>5</v>
+      </c>
+      <c r="H19" s="33">
+        <v>0</v>
+      </c>
+      <c r="I19" s="33">
+        <v>0</v>
+      </c>
+      <c r="J19" s="33">
+        <v>42</v>
+      </c>
+      <c r="K19" s="33">
+        <v>50</v>
+      </c>
+      <c r="L19" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20" s="33">
+        <v>11</v>
+      </c>
+      <c r="C20" s="33">
+        <v>0</v>
+      </c>
+      <c r="D20" s="33">
+        <v>0</v>
+      </c>
+      <c r="E20" s="33">
+        <v>0</v>
+      </c>
+      <c r="F20" s="33">
+        <v>1</v>
+      </c>
+      <c r="G20" s="33">
+        <v>2</v>
+      </c>
+      <c r="H20" s="33">
+        <v>0</v>
+      </c>
+      <c r="I20" s="33">
+        <v>0</v>
+      </c>
+      <c r="J20" s="33">
+        <v>54</v>
+      </c>
+      <c r="K20" s="33">
+        <v>66</v>
+      </c>
+      <c r="L20" s="33">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21" s="33">
+        <v>7</v>
+      </c>
+      <c r="C21" s="33">
+        <v>0</v>
+      </c>
+      <c r="D21" s="33">
+        <v>0</v>
+      </c>
+      <c r="E21" s="33">
+        <v>0</v>
+      </c>
+      <c r="F21" s="33">
+        <v>0</v>
+      </c>
+      <c r="G21" s="33">
+        <v>4</v>
+      </c>
+      <c r="H21" s="33">
+        <v>0</v>
+      </c>
+      <c r="I21" s="33">
+        <v>0</v>
+      </c>
+      <c r="J21" s="33">
+        <v>43</v>
+      </c>
+      <c r="K21" s="33">
+        <v>50</v>
+      </c>
+      <c r="L21" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="B22" s="33">
+        <v>8</v>
+      </c>
+      <c r="C22" s="33">
+        <v>0</v>
+      </c>
+      <c r="D22" s="33">
+        <v>0</v>
+      </c>
+      <c r="E22" s="33">
+        <v>0</v>
+      </c>
+      <c r="F22" s="33">
+        <v>0</v>
+      </c>
+      <c r="G22" s="33">
+        <v>3</v>
+      </c>
+      <c r="H22" s="33">
+        <v>0</v>
+      </c>
+      <c r="I22" s="33">
+        <v>0</v>
+      </c>
+      <c r="J22" s="33">
+        <v>42</v>
+      </c>
+      <c r="K22" s="33">
+        <v>50</v>
+      </c>
+      <c r="L22" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B23" s="33">
+        <v>6</v>
+      </c>
+      <c r="C23" s="33">
+        <v>0</v>
+      </c>
+      <c r="D23" s="33">
+        <v>0</v>
+      </c>
+      <c r="E23" s="33">
+        <v>0</v>
+      </c>
+      <c r="F23" s="33">
+        <v>0</v>
+      </c>
+      <c r="G23" s="33">
+        <v>2</v>
+      </c>
+      <c r="H23" s="33">
+        <v>0</v>
+      </c>
+      <c r="I23" s="33">
+        <v>0</v>
+      </c>
+      <c r="J23" s="33">
+        <v>44</v>
+      </c>
+      <c r="K23" s="33">
+        <v>50</v>
+      </c>
+      <c r="L23" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="B24" s="33">
+        <v>3</v>
+      </c>
+      <c r="C24" s="33">
+        <v>0</v>
+      </c>
+      <c r="D24" s="33">
+        <v>0</v>
+      </c>
+      <c r="E24" s="33">
+        <v>0</v>
+      </c>
+      <c r="F24" s="33">
+        <v>0</v>
+      </c>
+      <c r="G24" s="33">
+        <v>2</v>
+      </c>
+      <c r="H24" s="33">
+        <v>0</v>
+      </c>
+      <c r="I24" s="33">
+        <v>0</v>
+      </c>
+      <c r="J24" s="33">
+        <v>47</v>
+      </c>
+      <c r="K24" s="33">
+        <v>50</v>
+      </c>
+      <c r="L24" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25" s="33">
+        <v>15</v>
+      </c>
+      <c r="C25" s="33">
+        <v>1</v>
+      </c>
+      <c r="D25" s="33">
+        <v>0</v>
+      </c>
+      <c r="E25" s="33">
+        <v>0</v>
+      </c>
+      <c r="F25" s="33">
+        <v>1</v>
+      </c>
+      <c r="G25" s="33">
+        <v>7</v>
+      </c>
+      <c r="H25" s="33">
+        <v>0</v>
+      </c>
+      <c r="I25" s="33">
+        <v>0</v>
+      </c>
+      <c r="J25" s="33">
+        <v>60</v>
+      </c>
+      <c r="K25" s="33">
+        <v>75</v>
+      </c>
+      <c r="L25" s="33">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26" s="33">
+        <v>8</v>
+      </c>
+      <c r="C26" s="33">
+        <v>0</v>
+      </c>
+      <c r="D26" s="33">
+        <v>1</v>
+      </c>
+      <c r="E26" s="33">
+        <v>0</v>
+      </c>
+      <c r="F26" s="33">
+        <v>0</v>
+      </c>
+      <c r="G26" s="33">
+        <v>2</v>
+      </c>
+      <c r="H26" s="33">
+        <v>0</v>
+      </c>
+      <c r="I26" s="33">
+        <v>0</v>
+      </c>
+      <c r="J26" s="33">
+        <v>41</v>
+      </c>
+      <c r="K26" s="33">
+        <v>50</v>
+      </c>
+      <c r="L26" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="B27" s="33">
+        <v>5</v>
+      </c>
+      <c r="C27" s="33">
+        <v>0</v>
+      </c>
+      <c r="D27" s="33">
+        <v>2</v>
+      </c>
+      <c r="E27" s="33">
+        <v>0</v>
+      </c>
+      <c r="F27" s="33">
+        <v>0</v>
+      </c>
+      <c r="G27" s="33">
+        <v>5</v>
+      </c>
+      <c r="H27" s="33">
+        <v>0</v>
+      </c>
+      <c r="I27" s="33">
+        <v>0</v>
+      </c>
+      <c r="J27" s="33">
+        <v>43</v>
+      </c>
+      <c r="K27" s="33">
+        <v>50</v>
+      </c>
+      <c r="L27" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="B28" s="33">
+        <v>5</v>
+      </c>
+      <c r="C28" s="33">
+        <v>0</v>
+      </c>
+      <c r="D28" s="33">
+        <v>1</v>
+      </c>
+      <c r="E28" s="33">
+        <v>0</v>
+      </c>
+      <c r="F28" s="33">
+        <v>0</v>
+      </c>
+      <c r="G28" s="33">
+        <v>0</v>
+      </c>
+      <c r="H28" s="33">
+        <v>0</v>
+      </c>
+      <c r="I28" s="33">
+        <v>0</v>
+      </c>
+      <c r="J28" s="33">
+        <v>44</v>
+      </c>
+      <c r="K28" s="33">
+        <v>50</v>
+      </c>
+      <c r="L28" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="B29" s="33">
+        <v>6</v>
+      </c>
+      <c r="C29" s="33">
+        <v>0</v>
+      </c>
+      <c r="D29" s="33">
+        <v>0</v>
+      </c>
+      <c r="E29" s="33">
+        <v>0</v>
+      </c>
+      <c r="F29" s="33">
+        <v>0</v>
+      </c>
+      <c r="G29" s="33">
+        <v>1</v>
+      </c>
+      <c r="H29" s="33">
+        <v>0</v>
+      </c>
+      <c r="I29" s="33">
+        <v>0</v>
+      </c>
+      <c r="J29" s="33">
+        <v>44</v>
+      </c>
+      <c r="K29" s="33">
+        <v>50</v>
+      </c>
+      <c r="L29" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30" s="33">
+        <v>12</v>
+      </c>
+      <c r="C30" s="33">
+        <v>0</v>
+      </c>
+      <c r="D30" s="33">
+        <v>0</v>
+      </c>
+      <c r="E30" s="33">
+        <v>0</v>
+      </c>
+      <c r="F30" s="33">
+        <v>1</v>
+      </c>
+      <c r="G30" s="33">
+        <v>1</v>
+      </c>
+      <c r="H30" s="33">
+        <v>0</v>
+      </c>
+      <c r="I30" s="33">
+        <v>0</v>
+      </c>
+      <c r="J30" s="33">
+        <v>50</v>
+      </c>
+      <c r="K30" s="33">
+        <v>63</v>
+      </c>
+      <c r="L30" s="33">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="B31" s="33">
+        <v>14</v>
+      </c>
+      <c r="C31" s="33">
+        <v>0</v>
+      </c>
+      <c r="D31" s="33">
+        <v>0</v>
+      </c>
+      <c r="E31" s="33">
+        <v>0</v>
+      </c>
+      <c r="F31" s="33">
+        <v>0</v>
+      </c>
+      <c r="G31" s="33">
+        <v>5</v>
+      </c>
+      <c r="H31" s="33">
+        <v>0</v>
+      </c>
+      <c r="I31" s="33">
+        <v>0</v>
+      </c>
+      <c r="J31" s="33">
+        <v>36</v>
+      </c>
+      <c r="K31" s="33">
+        <v>50</v>
+      </c>
+      <c r="L31" s="33">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="B32" s="33">
+        <v>18</v>
+      </c>
+      <c r="C32" s="33">
+        <v>0</v>
+      </c>
+      <c r="D32" s="33">
+        <v>1</v>
+      </c>
+      <c r="E32" s="33">
+        <v>0</v>
+      </c>
+      <c r="F32" s="33">
+        <v>0</v>
+      </c>
+      <c r="G32" s="33">
+        <v>0</v>
+      </c>
+      <c r="H32" s="33">
+        <v>0</v>
+      </c>
+      <c r="I32" s="33">
+        <v>0</v>
+      </c>
+      <c r="J32" s="33">
+        <v>31</v>
+      </c>
+      <c r="K32" s="33">
+        <v>50</v>
+      </c>
+      <c r="L32" s="33">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="B33" s="33">
+        <v>14</v>
+      </c>
+      <c r="C33" s="33">
+        <v>0</v>
+      </c>
+      <c r="D33" s="33">
+        <v>0</v>
+      </c>
+      <c r="E33" s="33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="33">
+        <v>0</v>
+      </c>
+      <c r="G33" s="33">
+        <v>1</v>
+      </c>
+      <c r="H33" s="33">
+        <v>0</v>
+      </c>
+      <c r="I33" s="33">
+        <v>0</v>
+      </c>
+      <c r="J33" s="33">
+        <v>36</v>
+      </c>
+      <c r="K33" s="33">
+        <v>50</v>
+      </c>
+      <c r="L33" s="33">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B34" s="33">
+        <v>17</v>
+      </c>
+      <c r="C34" s="33">
+        <v>0</v>
+      </c>
+      <c r="D34" s="33">
+        <v>0</v>
+      </c>
+      <c r="E34" s="33">
+        <v>0</v>
+      </c>
+      <c r="F34" s="33">
+        <v>1</v>
+      </c>
+      <c r="G34" s="33">
+        <v>3</v>
+      </c>
+      <c r="H34" s="33">
+        <v>0</v>
+      </c>
+      <c r="I34" s="33">
+        <v>0</v>
+      </c>
+      <c r="J34" s="33">
+        <v>50</v>
+      </c>
+      <c r="K34" s="33">
+        <v>68</v>
+      </c>
+      <c r="L34" s="33">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" s="33">
+        <v>7</v>
+      </c>
+      <c r="C35" s="33">
+        <v>0</v>
+      </c>
+      <c r="D35" s="33">
+        <v>0</v>
+      </c>
+      <c r="E35" s="33">
+        <v>0</v>
+      </c>
+      <c r="F35" s="33">
+        <v>0</v>
+      </c>
+      <c r="G35" s="33">
+        <v>3</v>
+      </c>
+      <c r="H35" s="33">
+        <v>0</v>
+      </c>
+      <c r="I35" s="33">
+        <v>0</v>
+      </c>
+      <c r="J35" s="33">
+        <v>43</v>
+      </c>
+      <c r="K35" s="33">
+        <v>50</v>
+      </c>
+      <c r="L35" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="B36" s="33">
+        <v>2</v>
+      </c>
+      <c r="C36" s="33">
+        <v>0</v>
+      </c>
+      <c r="D36" s="33">
+        <v>1</v>
+      </c>
+      <c r="E36" s="33">
+        <v>0</v>
+      </c>
+      <c r="F36" s="33">
+        <v>0</v>
+      </c>
+      <c r="G36" s="33">
+        <v>1</v>
+      </c>
+      <c r="H36" s="33">
+        <v>0</v>
+      </c>
+      <c r="I36" s="33">
+        <v>0</v>
+      </c>
+      <c r="J36" s="33">
+        <v>47</v>
+      </c>
+      <c r="K36" s="33">
+        <v>50</v>
+      </c>
+      <c r="L36" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="B37" s="33">
+        <v>5</v>
+      </c>
+      <c r="C37" s="33">
+        <v>0</v>
+      </c>
+      <c r="D37" s="33">
+        <v>0</v>
+      </c>
+      <c r="E37" s="33">
+        <v>0</v>
+      </c>
+      <c r="F37" s="33">
+        <v>0</v>
+      </c>
+      <c r="G37" s="33">
+        <v>2</v>
+      </c>
+      <c r="H37" s="33">
+        <v>0</v>
+      </c>
+      <c r="I37" s="33">
+        <v>0</v>
+      </c>
+      <c r="J37" s="33">
+        <v>45</v>
+      </c>
+      <c r="K37" s="33">
+        <v>50</v>
+      </c>
+      <c r="L37" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="B38" s="33">
+        <v>8</v>
+      </c>
+      <c r="C38" s="33">
+        <v>0</v>
+      </c>
+      <c r="D38" s="33">
+        <v>0</v>
+      </c>
+      <c r="E38" s="33">
+        <v>0</v>
+      </c>
+      <c r="F38" s="33">
+        <v>0</v>
+      </c>
+      <c r="G38" s="33">
+        <v>7</v>
+      </c>
+      <c r="H38" s="33">
+        <v>0</v>
+      </c>
+      <c r="I38" s="33">
+        <v>0</v>
+      </c>
+      <c r="J38" s="33">
+        <v>42</v>
+      </c>
+      <c r="K38" s="33">
+        <v>50</v>
+      </c>
+      <c r="L38" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="B39" s="33">
+        <v>12</v>
+      </c>
+      <c r="C39" s="33">
+        <v>0</v>
+      </c>
+      <c r="D39" s="33">
+        <v>0</v>
+      </c>
+      <c r="E39" s="33">
+        <v>0</v>
+      </c>
+      <c r="F39" s="33">
+        <v>1</v>
+      </c>
+      <c r="G39" s="33">
+        <v>3</v>
+      </c>
+      <c r="H39" s="33">
+        <v>0</v>
+      </c>
+      <c r="I39" s="33">
+        <v>0</v>
+      </c>
+      <c r="J39" s="33">
+        <v>40</v>
+      </c>
+      <c r="K39" s="33">
+        <v>53</v>
+      </c>
+      <c r="L39" s="33">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="B40" s="33">
+        <v>7</v>
+      </c>
+      <c r="C40" s="33">
+        <v>0</v>
+      </c>
+      <c r="D40" s="33">
+        <v>0</v>
+      </c>
+      <c r="E40" s="33">
+        <v>0</v>
+      </c>
+      <c r="F40" s="33">
+        <v>0</v>
+      </c>
+      <c r="G40" s="33">
+        <v>3</v>
+      </c>
+      <c r="H40" s="33">
+        <v>0</v>
+      </c>
+      <c r="I40" s="33">
+        <v>0</v>
+      </c>
+      <c r="J40" s="33">
+        <v>43</v>
+      </c>
+      <c r="K40" s="33">
+        <v>50</v>
+      </c>
+      <c r="L40" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="B41" s="33">
+        <v>7</v>
+      </c>
+      <c r="C41" s="33">
+        <v>0</v>
+      </c>
+      <c r="D41" s="33">
+        <v>0</v>
+      </c>
+      <c r="E41" s="33">
+        <v>0</v>
+      </c>
+      <c r="F41" s="33">
+        <v>0</v>
+      </c>
+      <c r="G41" s="33">
+        <v>2</v>
+      </c>
+      <c r="H41" s="33">
+        <v>0</v>
+      </c>
+      <c r="I41" s="33">
+        <v>0</v>
+      </c>
+      <c r="J41" s="33">
+        <v>43</v>
+      </c>
+      <c r="K41" s="33">
+        <v>50</v>
+      </c>
+      <c r="L41" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="B42" s="33">
+        <v>7</v>
+      </c>
+      <c r="C42" s="33">
+        <v>0</v>
+      </c>
+      <c r="D42" s="33">
+        <v>0</v>
+      </c>
+      <c r="E42" s="33">
+        <v>0</v>
+      </c>
+      <c r="F42" s="33">
+        <v>0</v>
+      </c>
+      <c r="G42" s="33">
+        <v>5</v>
+      </c>
+      <c r="H42" s="33">
+        <v>0</v>
+      </c>
+      <c r="I42" s="33">
+        <v>0</v>
+      </c>
+      <c r="J42" s="33">
+        <v>43</v>
+      </c>
+      <c r="K42" s="33">
+        <v>50</v>
+      </c>
+      <c r="L42" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="B43" s="33">
+        <v>3</v>
+      </c>
+      <c r="C43" s="33">
+        <v>0</v>
+      </c>
+      <c r="D43" s="33">
+        <v>1</v>
+      </c>
+      <c r="E43" s="33">
+        <v>0</v>
+      </c>
+      <c r="F43" s="33">
+        <v>0</v>
+      </c>
+      <c r="G43" s="33">
+        <v>3</v>
+      </c>
+      <c r="H43" s="33">
+        <v>0</v>
+      </c>
+      <c r="I43" s="33">
+        <v>0</v>
+      </c>
+      <c r="J43" s="33">
+        <v>46</v>
+      </c>
+      <c r="K43" s="33">
+        <v>50</v>
+      </c>
+      <c r="L43" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="B44" s="33">
+        <v>5</v>
+      </c>
+      <c r="C44" s="33">
+        <v>0</v>
+      </c>
+      <c r="D44" s="33">
+        <v>0</v>
+      </c>
+      <c r="E44" s="33">
+        <v>0</v>
+      </c>
+      <c r="F44" s="33">
+        <v>0</v>
+      </c>
+      <c r="G44" s="33">
+        <v>3</v>
+      </c>
+      <c r="H44" s="33">
+        <v>0</v>
+      </c>
+      <c r="I44" s="33">
+        <v>0</v>
+      </c>
+      <c r="J44" s="33">
+        <v>45</v>
+      </c>
+      <c r="K44" s="33">
+        <v>50</v>
+      </c>
+      <c r="L44" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B45" s="33">
+        <v>5</v>
+      </c>
+      <c r="C45" s="33">
+        <v>0</v>
+      </c>
+      <c r="D45" s="33">
+        <v>1</v>
+      </c>
+      <c r="E45" s="33">
+        <v>0</v>
+      </c>
+      <c r="F45" s="33">
+        <v>1</v>
+      </c>
+      <c r="G45" s="33">
+        <v>2</v>
+      </c>
+      <c r="H45" s="33">
+        <v>0</v>
+      </c>
+      <c r="I45" s="33">
+        <v>0</v>
+      </c>
+      <c r="J45" s="33">
+        <v>37</v>
+      </c>
+      <c r="K45" s="33">
+        <v>44</v>
+      </c>
+      <c r="L45" s="33">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="B46" s="33">
+        <v>6</v>
+      </c>
+      <c r="C46" s="33">
+        <v>0</v>
+      </c>
+      <c r="D46" s="33">
+        <v>5</v>
+      </c>
+      <c r="E46" s="33">
+        <v>0</v>
+      </c>
+      <c r="F46" s="33">
+        <v>0</v>
+      </c>
+      <c r="G46" s="33">
+        <v>5</v>
+      </c>
+      <c r="H46" s="33">
+        <v>0</v>
+      </c>
+      <c r="I46" s="33">
+        <v>0</v>
+      </c>
+      <c r="J46" s="33">
+        <v>39</v>
+      </c>
+      <c r="K46" s="33">
+        <v>50</v>
+      </c>
+      <c r="L46" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="B47" s="33">
+        <v>6</v>
+      </c>
+      <c r="C47" s="33">
+        <v>0</v>
+      </c>
+      <c r="D47" s="33">
+        <v>1</v>
+      </c>
+      <c r="E47" s="33">
+        <v>0</v>
+      </c>
+      <c r="F47" s="33">
+        <v>0</v>
+      </c>
+      <c r="G47" s="33">
+        <v>2</v>
+      </c>
+      <c r="H47" s="33">
+        <v>0</v>
+      </c>
+      <c r="I47" s="33">
+        <v>0</v>
+      </c>
+      <c r="J47" s="33">
+        <v>43</v>
+      </c>
+      <c r="K47" s="33">
+        <v>50</v>
+      </c>
+      <c r="L47" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="B48" s="33">
+        <v>5</v>
+      </c>
+      <c r="C48" s="33">
+        <v>0</v>
+      </c>
+      <c r="D48" s="33">
+        <v>3</v>
+      </c>
+      <c r="E48" s="33">
+        <v>0</v>
+      </c>
+      <c r="F48" s="33">
+        <v>0</v>
+      </c>
+      <c r="G48" s="33">
+        <v>1</v>
+      </c>
+      <c r="H48" s="33">
+        <v>0</v>
+      </c>
+      <c r="I48" s="33">
+        <v>0</v>
+      </c>
+      <c r="J48" s="33">
+        <v>42</v>
+      </c>
+      <c r="K48" s="33">
+        <v>50</v>
+      </c>
+      <c r="L48" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B49" s="33">
+        <v>15</v>
+      </c>
+      <c r="C49" s="33">
+        <v>1</v>
+      </c>
+      <c r="D49" s="33">
+        <v>0</v>
+      </c>
+      <c r="E49" s="33">
+        <v>0</v>
+      </c>
+      <c r="F49" s="33">
+        <v>1</v>
+      </c>
+      <c r="G49" s="33">
+        <v>3</v>
+      </c>
+      <c r="H49" s="33">
+        <v>0</v>
+      </c>
+      <c r="I49" s="33">
+        <v>0</v>
+      </c>
+      <c r="J49" s="33">
+        <v>61</v>
+      </c>
+      <c r="K49" s="33">
+        <v>76</v>
+      </c>
+      <c r="L49" s="33">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="B50" s="33">
+        <v>7</v>
+      </c>
+      <c r="C50" s="33">
+        <v>0</v>
+      </c>
+      <c r="D50" s="33">
+        <v>1</v>
+      </c>
+      <c r="E50" s="33">
+        <v>0</v>
+      </c>
+      <c r="F50" s="33">
+        <v>0</v>
+      </c>
+      <c r="G50" s="33">
+        <v>1</v>
+      </c>
+      <c r="H50" s="33">
+        <v>0</v>
+      </c>
+      <c r="I50" s="33">
+        <v>0</v>
+      </c>
+      <c r="J50" s="33">
+        <v>42</v>
+      </c>
+      <c r="K50" s="33">
+        <v>50</v>
+      </c>
+      <c r="L50" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="B51" s="33">
+        <v>1</v>
+      </c>
+      <c r="C51" s="33">
+        <v>0</v>
+      </c>
+      <c r="D51" s="33">
+        <v>0</v>
+      </c>
+      <c r="E51" s="33">
+        <v>0</v>
+      </c>
+      <c r="F51" s="33">
+        <v>0</v>
+      </c>
+      <c r="G51" s="33">
+        <v>3</v>
+      </c>
+      <c r="H51" s="33">
+        <v>0</v>
+      </c>
+      <c r="I51" s="33">
+        <v>0</v>
+      </c>
+      <c r="J51" s="33">
+        <v>49</v>
+      </c>
+      <c r="K51" s="33">
+        <v>50</v>
+      </c>
+      <c r="L51" s="33">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="B52" s="33">
+        <v>3</v>
+      </c>
+      <c r="C52" s="33">
+        <v>0</v>
+      </c>
+      <c r="D52" s="33">
+        <v>0</v>
+      </c>
+      <c r="E52" s="33">
+        <v>0</v>
+      </c>
+      <c r="F52" s="33">
+        <v>0</v>
+      </c>
+      <c r="G52" s="33">
+        <v>5</v>
+      </c>
+      <c r="H52" s="33">
+        <v>0</v>
+      </c>
+      <c r="I52" s="33">
+        <v>0</v>
+      </c>
+      <c r="J52" s="33">
+        <v>47</v>
+      </c>
+      <c r="K52" s="33">
+        <v>50</v>
+      </c>
+      <c r="L52" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="B53" s="33">
+        <v>7</v>
+      </c>
+      <c r="C53" s="33">
+        <v>0</v>
+      </c>
+      <c r="D53" s="33">
+        <v>1</v>
+      </c>
+      <c r="E53" s="33">
+        <v>0</v>
+      </c>
+      <c r="F53" s="33">
+        <v>0</v>
+      </c>
+      <c r="G53" s="33">
+        <v>2</v>
+      </c>
+      <c r="H53" s="33">
+        <v>0</v>
+      </c>
+      <c r="I53" s="33">
+        <v>0</v>
+      </c>
+      <c r="J53" s="33">
+        <v>42</v>
+      </c>
+      <c r="K53" s="33">
+        <v>50</v>
+      </c>
+      <c r="L53" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="B54" s="33">
+        <v>9</v>
+      </c>
+      <c r="C54" s="33">
+        <v>0</v>
+      </c>
+      <c r="D54" s="33">
+        <v>2</v>
+      </c>
+      <c r="E54" s="33">
+        <v>0</v>
+      </c>
+      <c r="F54" s="33">
+        <v>0</v>
+      </c>
+      <c r="G54" s="33">
+        <v>3</v>
+      </c>
+      <c r="H54" s="33">
+        <v>0</v>
+      </c>
+      <c r="I54" s="33">
+        <v>0</v>
+      </c>
+      <c r="J54" s="33">
+        <v>39</v>
+      </c>
+      <c r="K54" s="33">
+        <v>50</v>
+      </c>
+      <c r="L54" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="B55" s="33">
+        <v>22</v>
+      </c>
+      <c r="C55" s="33">
+        <v>0</v>
+      </c>
+      <c r="D55" s="33">
+        <v>0</v>
+      </c>
+      <c r="E55" s="33">
+        <v>0</v>
+      </c>
+      <c r="F55" s="33">
+        <v>0</v>
+      </c>
+      <c r="G55" s="33">
+        <v>0</v>
+      </c>
+      <c r="H55" s="33">
+        <v>0</v>
+      </c>
+      <c r="I55" s="33">
+        <v>0</v>
+      </c>
+      <c r="J55" s="33">
+        <v>28</v>
+      </c>
+      <c r="K55" s="33">
+        <v>50</v>
+      </c>
+      <c r="L55" s="33">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="B56" s="33">
+        <v>12</v>
+      </c>
+      <c r="C56" s="33">
+        <v>1</v>
+      </c>
+      <c r="D56" s="33">
+        <v>0</v>
+      </c>
+      <c r="E56" s="33">
+        <v>0</v>
+      </c>
+      <c r="F56" s="33">
+        <v>1</v>
+      </c>
+      <c r="G56" s="33">
+        <v>3</v>
+      </c>
+      <c r="H56" s="33">
+        <v>0</v>
+      </c>
+      <c r="I56" s="33">
+        <v>0</v>
+      </c>
+      <c r="J56" s="33">
+        <v>53</v>
+      </c>
+      <c r="K56" s="33">
+        <v>65</v>
+      </c>
+      <c r="L56" s="33">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="B57" s="33">
+        <v>15</v>
+      </c>
+      <c r="C57" s="33">
+        <v>0</v>
+      </c>
+      <c r="D57" s="33">
+        <v>0</v>
+      </c>
+      <c r="E57" s="33">
+        <v>0</v>
+      </c>
+      <c r="F57" s="33">
+        <v>0</v>
+      </c>
+      <c r="G57" s="33">
+        <v>3</v>
+      </c>
+      <c r="H57" s="33">
+        <v>0</v>
+      </c>
+      <c r="I57" s="33">
+        <v>0</v>
+      </c>
+      <c r="J57" s="33">
+        <v>35</v>
+      </c>
+      <c r="K57" s="33">
+        <v>50</v>
+      </c>
+      <c r="L57" s="33">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="B58" s="33">
+        <v>9</v>
+      </c>
+      <c r="C58" s="33">
+        <v>0</v>
+      </c>
+      <c r="D58" s="33">
+        <v>0</v>
+      </c>
+      <c r="E58" s="33">
+        <v>0</v>
+      </c>
+      <c r="F58" s="33">
+        <v>0</v>
+      </c>
+      <c r="G58" s="33">
+        <v>5</v>
+      </c>
+      <c r="H58" s="33">
+        <v>0</v>
+      </c>
+      <c r="I58" s="33">
+        <v>0</v>
+      </c>
+      <c r="J58" s="33">
+        <v>41</v>
+      </c>
+      <c r="K58" s="33">
+        <v>50</v>
+      </c>
+      <c r="L58" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="B59" s="33">
+        <v>10</v>
+      </c>
+      <c r="C59" s="33">
+        <v>0</v>
+      </c>
+      <c r="D59" s="33">
+        <v>7</v>
+      </c>
+      <c r="E59" s="33">
+        <v>0</v>
+      </c>
+      <c r="F59" s="33">
+        <v>0</v>
+      </c>
+      <c r="G59" s="33">
+        <v>2</v>
+      </c>
+      <c r="H59" s="33">
+        <v>0</v>
+      </c>
+      <c r="I59" s="33">
+        <v>0</v>
+      </c>
+      <c r="J59" s="33">
+        <v>33</v>
+      </c>
+      <c r="K59" s="33">
+        <v>50</v>
+      </c>
+      <c r="L59" s="33">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="B60" s="33">
+        <v>13</v>
+      </c>
+      <c r="C60" s="33">
+        <v>0</v>
+      </c>
+      <c r="D60" s="33">
+        <v>4</v>
+      </c>
+      <c r="E60" s="33">
+        <v>0</v>
+      </c>
+      <c r="F60" s="33">
+        <v>1</v>
+      </c>
+      <c r="G60" s="33">
+        <v>2</v>
+      </c>
+      <c r="H60" s="33">
+        <v>0</v>
+      </c>
+      <c r="I60" s="33">
+        <v>0</v>
+      </c>
+      <c r="J60" s="33">
+        <v>55</v>
+      </c>
+      <c r="K60" s="33">
+        <v>73</v>
+      </c>
+      <c r="L60" s="33">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="B61" s="36">
+        <f>SUM(B2:B60)</f>
+        <v>505</v>
+      </c>
+      <c r="C61" s="36">
+        <f>SUM(C2:C60)</f>
+        <v>3</v>
+      </c>
+      <c r="D61" s="36">
+        <f>SUM(D2:D60)</f>
+        <v>41</v>
+      </c>
+      <c r="E61" s="36">
+        <f>SUM(E2:E60)</f>
+        <v>0</v>
+      </c>
+      <c r="F61" s="36">
+        <f>SUM(F2:F60)</f>
+        <v>11</v>
+      </c>
+      <c r="G61" s="36">
+        <f>SUM(G2:G60)</f>
+        <v>157</v>
+      </c>
+      <c r="H61" s="36">
+        <f t="shared" ref="H61:L61" si="0">SUM(H2:H60)</f>
+        <v>0</v>
+      </c>
+      <c r="I61" s="36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J61" s="36">
+        <f t="shared" si="0"/>
+        <v>2531</v>
+      </c>
+      <c r="K61" s="36">
+        <f t="shared" si="0"/>
+        <v>3085</v>
+      </c>
+      <c r="L61" s="36">
+        <f t="shared" si="0"/>
+        <v>3628</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>39</v>
+      </c>
+      <c r="F62">
+        <f>G61</f>
+        <v>157</v>
+      </c>
+      <c r="J62">
+        <f>B61-C61</f>
+        <v>502</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>40</v>
+      </c>
+      <c r="F63">
+        <f>B61</f>
+        <v>505</v>
+      </c>
+      <c r="J63">
+        <f>D61-E61</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>41</v>
+      </c>
+      <c r="F64">
+        <v>31</v>
+      </c>
+      <c r="J64">
+        <f>F70</f>
+        <v>3085</v>
+      </c>
+    </row>
+    <row r="65" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>42</v>
+      </c>
+      <c r="F65">
+        <v>10</v>
+      </c>
+      <c r="J65" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="66" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F66" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="J66">
+        <f>SUM(J62:J65)</f>
+        <v>3628</v>
+      </c>
+    </row>
+    <row r="67" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <f>SUM(F62:F66)</f>
+        <v>703</v>
+      </c>
+      <c r="J67" s="35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="68" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>45</v>
+      </c>
+      <c r="F68">
+        <f>K61-F67</f>
+        <v>2382</v>
+      </c>
+      <c r="J68">
+        <f>J66-L61</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F69" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <f>F68+F67</f>
+        <v>3085</v>
+      </c>
+    </row>
+    <row r="71" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <f>F70-K61</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:K31"/>
   <sheetViews>
@@ -5341,7 +7979,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
nmv 08 11 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 6.1 TO 6.6.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 6.1 TO 6.6.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504E3982-D800-4F18-996B-D3D54E95A974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9EDA1D-39EA-4B26-9598-BCD11375EBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="6.1" sheetId="15" r:id="rId1"/>
     <sheet name="6.2" sheetId="16" r:id="rId2"/>
-    <sheet name="total 6.1 to 6.6" sheetId="7" r:id="rId3"/>
+    <sheet name="6.3" sheetId="17" r:id="rId3"/>
+    <sheet name="total 6.1 to 6.6" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="253">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -1802,6 +1803,195 @@
   </si>
   <si>
     <t>59</t>
+  </si>
+  <si>
+    <t>6.3.1.1 :</t>
+  </si>
+  <si>
+    <t>6.3.1.2 :</t>
+  </si>
+  <si>
+    <t>6.3.1.3 :</t>
+  </si>
+  <si>
+    <t>6.3.1.4 :</t>
+  </si>
+  <si>
+    <t>6.3.1.5 :</t>
+  </si>
+  <si>
+    <t>6.3.1.6 :</t>
+  </si>
+  <si>
+    <t>6.3.2.1 :</t>
+  </si>
+  <si>
+    <t>6.3.2.2 :</t>
+  </si>
+  <si>
+    <t>6.3.2.3 :</t>
+  </si>
+  <si>
+    <t>6.3.2.4 :</t>
+  </si>
+  <si>
+    <t>6.3.2.5 :</t>
+  </si>
+  <si>
+    <t>6.3.2.6 :</t>
+  </si>
+  <si>
+    <t>6.3.3.1 :</t>
+  </si>
+  <si>
+    <t>6.3.3.2 :</t>
+  </si>
+  <si>
+    <t>6.3.3.3 :</t>
+  </si>
+  <si>
+    <t>6.3.3.4 :</t>
+  </si>
+  <si>
+    <t>6.3.3.5 :</t>
+  </si>
+  <si>
+    <t>6.3.3.6 :</t>
+  </si>
+  <si>
+    <t>6.3.4.1 :</t>
+  </si>
+  <si>
+    <t>6.3.4.2 :</t>
+  </si>
+  <si>
+    <t>6.3.4.3 :</t>
+  </si>
+  <si>
+    <t>6.3.4.4 :</t>
+  </si>
+  <si>
+    <t>6.3.4.5 :</t>
+  </si>
+  <si>
+    <t>6.3.4.6 :</t>
+  </si>
+  <si>
+    <t>6.3.4.7 :</t>
+  </si>
+  <si>
+    <t>6.3.4.8 :</t>
+  </si>
+  <si>
+    <t>6.3.4.9 :</t>
+  </si>
+  <si>
+    <t>6.3.5.1 :</t>
+  </si>
+  <si>
+    <t>6.3.5.2 :</t>
+  </si>
+  <si>
+    <t>6.3.5.3 :</t>
+  </si>
+  <si>
+    <t>6.3.5.4 :</t>
+  </si>
+  <si>
+    <t>6.3.6.1 :</t>
+  </si>
+  <si>
+    <t>6.3.6.2 :</t>
+  </si>
+  <si>
+    <t>6.3.6.3 :</t>
+  </si>
+  <si>
+    <t>6.3.6.4 :</t>
+  </si>
+  <si>
+    <t>6.3.7.1 :</t>
+  </si>
+  <si>
+    <t>6.3.7.2 :</t>
+  </si>
+  <si>
+    <t>6.3.7.3 :</t>
+  </si>
+  <si>
+    <t>6.3.7.4 :</t>
+  </si>
+  <si>
+    <t>6.3.7.5 :</t>
+  </si>
+  <si>
+    <t>6.3.8.1 :</t>
+  </si>
+  <si>
+    <t>6.3.8.2 :</t>
+  </si>
+  <si>
+    <t>6.3.8.3 :</t>
+  </si>
+  <si>
+    <t>6.3.8.4 :</t>
+  </si>
+  <si>
+    <t>6.3.9.1 :</t>
+  </si>
+  <si>
+    <t>6.3.9.2 :</t>
+  </si>
+  <si>
+    <t>6.3.9.3 :</t>
+  </si>
+  <si>
+    <t>6.3.9.4 :</t>
+  </si>
+  <si>
+    <t>6.3.9.5 :</t>
+  </si>
+  <si>
+    <t>6.3.9.6 :</t>
+  </si>
+  <si>
+    <t>6.3.10.1 :</t>
+  </si>
+  <si>
+    <t>6.3.10.2 :</t>
+  </si>
+  <si>
+    <t>6.3.10.3 :</t>
+  </si>
+  <si>
+    <t>6.3.10.4 :</t>
+  </si>
+  <si>
+    <t>6.3.10.5 :</t>
+  </si>
+  <si>
+    <t>6.3.10.6 :</t>
+  </si>
+  <si>
+    <t>6.3.11.1 :</t>
+  </si>
+  <si>
+    <t>6.3.11.2 :</t>
+  </si>
+  <si>
+    <t>6.3.11.3 :</t>
+  </si>
+  <si>
+    <t>6.3.11.4 :</t>
+  </si>
+  <si>
+    <t>6.3.11.5 :</t>
+  </si>
+  <si>
+    <t>6.3.11.6 :</t>
+  </si>
+  <si>
+    <t>62</t>
   </si>
 </sst>
 </file>
@@ -5480,9 +5670,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D38C19-8B03-4797-B383-C63371C35E12}">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M65" sqref="M65"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D62" sqref="D62:J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7784,47 +7974,47 @@
         <v>189</v>
       </c>
       <c r="B61" s="36">
-        <f>SUM(B2:B60)</f>
+        <f t="shared" ref="B61:G61" si="0">SUM(B2:B60)</f>
         <v>505</v>
       </c>
       <c r="C61" s="36">
-        <f>SUM(C2:C60)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D61" s="36">
-        <f>SUM(D2:D60)</f>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="E61" s="36">
-        <f>SUM(E2:E60)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F61" s="36">
-        <f>SUM(F2:F60)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G61" s="36">
-        <f>SUM(G2:G60)</f>
+        <f t="shared" si="0"/>
         <v>157</v>
       </c>
       <c r="H61" s="36">
-        <f t="shared" ref="H61:L61" si="0">SUM(H2:H60)</f>
+        <f t="shared" ref="H61:L61" si="1">SUM(H2:H60)</f>
         <v>0</v>
       </c>
       <c r="I61" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J61" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2531</v>
       </c>
       <c r="K61" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3085</v>
       </c>
       <c r="L61" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3628</v>
       </c>
     </row>
@@ -7931,6 +8121,2574 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02ADB140-5197-4869-A498-C69E75D5151E}">
+  <dimension ref="A1:L74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:L64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="33">
+        <v>10</v>
+      </c>
+      <c r="C2" s="33">
+        <v>0</v>
+      </c>
+      <c r="D2" s="33">
+        <v>0</v>
+      </c>
+      <c r="E2" s="33">
+        <v>0</v>
+      </c>
+      <c r="F2" s="33">
+        <v>0</v>
+      </c>
+      <c r="G2" s="33">
+        <v>3</v>
+      </c>
+      <c r="H2" s="33">
+        <v>0</v>
+      </c>
+      <c r="I2" s="33">
+        <v>0</v>
+      </c>
+      <c r="J2" s="33">
+        <v>40</v>
+      </c>
+      <c r="K2" s="33">
+        <v>50</v>
+      </c>
+      <c r="L2" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="33">
+        <v>4</v>
+      </c>
+      <c r="C3" s="33">
+        <v>0</v>
+      </c>
+      <c r="D3" s="33">
+        <v>3</v>
+      </c>
+      <c r="E3" s="33">
+        <v>0</v>
+      </c>
+      <c r="F3" s="33">
+        <v>0</v>
+      </c>
+      <c r="G3" s="33">
+        <v>6</v>
+      </c>
+      <c r="H3" s="33">
+        <v>0</v>
+      </c>
+      <c r="I3" s="33">
+        <v>0</v>
+      </c>
+      <c r="J3" s="33">
+        <v>43</v>
+      </c>
+      <c r="K3" s="33">
+        <v>50</v>
+      </c>
+      <c r="L3" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" s="33">
+        <v>9</v>
+      </c>
+      <c r="C4" s="33">
+        <v>0</v>
+      </c>
+      <c r="D4" s="33">
+        <v>2</v>
+      </c>
+      <c r="E4" s="33">
+        <v>0</v>
+      </c>
+      <c r="F4" s="33">
+        <v>0</v>
+      </c>
+      <c r="G4" s="33">
+        <v>4</v>
+      </c>
+      <c r="H4" s="33">
+        <v>0</v>
+      </c>
+      <c r="I4" s="33">
+        <v>0</v>
+      </c>
+      <c r="J4" s="33">
+        <v>39</v>
+      </c>
+      <c r="K4" s="33">
+        <v>50</v>
+      </c>
+      <c r="L4" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5" s="33">
+        <v>5</v>
+      </c>
+      <c r="C5" s="33">
+        <v>0</v>
+      </c>
+      <c r="D5" s="33">
+        <v>0</v>
+      </c>
+      <c r="E5" s="33">
+        <v>0</v>
+      </c>
+      <c r="F5" s="33">
+        <v>0</v>
+      </c>
+      <c r="G5" s="33">
+        <v>4</v>
+      </c>
+      <c r="H5" s="33">
+        <v>0</v>
+      </c>
+      <c r="I5" s="33">
+        <v>0</v>
+      </c>
+      <c r="J5" s="33">
+        <v>45</v>
+      </c>
+      <c r="K5" s="33">
+        <v>50</v>
+      </c>
+      <c r="L5" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="B6" s="33">
+        <v>13</v>
+      </c>
+      <c r="C6" s="33">
+        <v>0</v>
+      </c>
+      <c r="D6" s="33">
+        <v>0</v>
+      </c>
+      <c r="E6" s="33">
+        <v>0</v>
+      </c>
+      <c r="F6" s="33">
+        <v>0</v>
+      </c>
+      <c r="G6" s="33">
+        <v>2</v>
+      </c>
+      <c r="H6" s="33">
+        <v>0</v>
+      </c>
+      <c r="I6" s="33">
+        <v>0</v>
+      </c>
+      <c r="J6" s="33">
+        <v>37</v>
+      </c>
+      <c r="K6" s="33">
+        <v>50</v>
+      </c>
+      <c r="L6" s="33">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="B7" s="33">
+        <v>10</v>
+      </c>
+      <c r="C7" s="33">
+        <v>0</v>
+      </c>
+      <c r="D7" s="33">
+        <v>0</v>
+      </c>
+      <c r="E7" s="33">
+        <v>0</v>
+      </c>
+      <c r="F7" s="33">
+        <v>1</v>
+      </c>
+      <c r="G7" s="33">
+        <v>6</v>
+      </c>
+      <c r="H7" s="33">
+        <v>0</v>
+      </c>
+      <c r="I7" s="33">
+        <v>0</v>
+      </c>
+      <c r="J7" s="33">
+        <v>53</v>
+      </c>
+      <c r="K7" s="33">
+        <v>64</v>
+      </c>
+      <c r="L7" s="33">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="B8" s="33">
+        <v>11</v>
+      </c>
+      <c r="C8" s="33">
+        <v>0</v>
+      </c>
+      <c r="D8" s="33">
+        <v>0</v>
+      </c>
+      <c r="E8" s="33">
+        <v>0</v>
+      </c>
+      <c r="F8" s="33">
+        <v>0</v>
+      </c>
+      <c r="G8" s="33">
+        <v>1</v>
+      </c>
+      <c r="H8" s="33">
+        <v>0</v>
+      </c>
+      <c r="I8" s="33">
+        <v>0</v>
+      </c>
+      <c r="J8" s="33">
+        <v>39</v>
+      </c>
+      <c r="K8" s="33">
+        <v>50</v>
+      </c>
+      <c r="L8" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="B9" s="33">
+        <v>8</v>
+      </c>
+      <c r="C9" s="33">
+        <v>0</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0</v>
+      </c>
+      <c r="E9" s="33">
+        <v>0</v>
+      </c>
+      <c r="F9" s="33">
+        <v>0</v>
+      </c>
+      <c r="G9" s="33">
+        <v>1</v>
+      </c>
+      <c r="H9" s="33">
+        <v>0</v>
+      </c>
+      <c r="I9" s="33">
+        <v>0</v>
+      </c>
+      <c r="J9" s="33">
+        <v>42</v>
+      </c>
+      <c r="K9" s="33">
+        <v>50</v>
+      </c>
+      <c r="L9" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="B10" s="33">
+        <v>9</v>
+      </c>
+      <c r="C10" s="33">
+        <v>0</v>
+      </c>
+      <c r="D10" s="33">
+        <v>0</v>
+      </c>
+      <c r="E10" s="33">
+        <v>0</v>
+      </c>
+      <c r="F10" s="33">
+        <v>0</v>
+      </c>
+      <c r="G10" s="33">
+        <v>10</v>
+      </c>
+      <c r="H10" s="33">
+        <v>0</v>
+      </c>
+      <c r="I10" s="33">
+        <v>0</v>
+      </c>
+      <c r="J10" s="33">
+        <v>41</v>
+      </c>
+      <c r="K10" s="33">
+        <v>50</v>
+      </c>
+      <c r="L10" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="B11" s="33">
+        <v>2</v>
+      </c>
+      <c r="C11" s="33">
+        <v>0</v>
+      </c>
+      <c r="D11" s="33">
+        <v>0</v>
+      </c>
+      <c r="E11" s="33">
+        <v>0</v>
+      </c>
+      <c r="F11" s="33">
+        <v>0</v>
+      </c>
+      <c r="G11" s="33">
+        <v>5</v>
+      </c>
+      <c r="H11" s="33">
+        <v>0</v>
+      </c>
+      <c r="I11" s="33">
+        <v>0</v>
+      </c>
+      <c r="J11" s="33">
+        <v>48</v>
+      </c>
+      <c r="K11" s="33">
+        <v>50</v>
+      </c>
+      <c r="L11" s="33">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="B12" s="33">
+        <v>11</v>
+      </c>
+      <c r="C12" s="33">
+        <v>0</v>
+      </c>
+      <c r="D12" s="33">
+        <v>0</v>
+      </c>
+      <c r="E12" s="33">
+        <v>0</v>
+      </c>
+      <c r="F12" s="33">
+        <v>0</v>
+      </c>
+      <c r="G12" s="33">
+        <v>0</v>
+      </c>
+      <c r="H12" s="33">
+        <v>0</v>
+      </c>
+      <c r="I12" s="33">
+        <v>0</v>
+      </c>
+      <c r="J12" s="33">
+        <v>39</v>
+      </c>
+      <c r="K12" s="33">
+        <v>50</v>
+      </c>
+      <c r="L12" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="B13" s="33">
+        <v>7</v>
+      </c>
+      <c r="C13" s="33">
+        <v>0</v>
+      </c>
+      <c r="D13" s="33">
+        <v>0</v>
+      </c>
+      <c r="E13" s="33">
+        <v>0</v>
+      </c>
+      <c r="F13" s="33">
+        <v>1</v>
+      </c>
+      <c r="G13" s="33">
+        <v>2</v>
+      </c>
+      <c r="H13" s="33">
+        <v>0</v>
+      </c>
+      <c r="I13" s="33">
+        <v>0</v>
+      </c>
+      <c r="J13" s="33">
+        <v>42</v>
+      </c>
+      <c r="K13" s="33">
+        <v>50</v>
+      </c>
+      <c r="L13" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>202</v>
+      </c>
+      <c r="B14" s="33">
+        <v>1</v>
+      </c>
+      <c r="C14" s="33">
+        <v>0</v>
+      </c>
+      <c r="D14" s="33">
+        <v>0</v>
+      </c>
+      <c r="E14" s="33">
+        <v>0</v>
+      </c>
+      <c r="F14" s="33">
+        <v>0</v>
+      </c>
+      <c r="G14" s="33">
+        <v>3</v>
+      </c>
+      <c r="H14" s="33">
+        <v>0</v>
+      </c>
+      <c r="I14" s="33">
+        <v>0</v>
+      </c>
+      <c r="J14" s="33">
+        <v>49</v>
+      </c>
+      <c r="K14" s="33">
+        <v>50</v>
+      </c>
+      <c r="L14" s="33">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" s="33">
+        <v>7</v>
+      </c>
+      <c r="C15" s="33">
+        <v>0</v>
+      </c>
+      <c r="D15" s="33">
+        <v>0</v>
+      </c>
+      <c r="E15" s="33">
+        <v>0</v>
+      </c>
+      <c r="F15" s="33">
+        <v>0</v>
+      </c>
+      <c r="G15" s="33">
+        <v>3</v>
+      </c>
+      <c r="H15" s="33">
+        <v>0</v>
+      </c>
+      <c r="I15" s="33">
+        <v>0</v>
+      </c>
+      <c r="J15" s="33">
+        <v>43</v>
+      </c>
+      <c r="K15" s="33">
+        <v>50</v>
+      </c>
+      <c r="L15" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="B16" s="33">
+        <v>7</v>
+      </c>
+      <c r="C16" s="33">
+        <v>0</v>
+      </c>
+      <c r="D16" s="33">
+        <v>0</v>
+      </c>
+      <c r="E16" s="33">
+        <v>0</v>
+      </c>
+      <c r="F16" s="33">
+        <v>0</v>
+      </c>
+      <c r="G16" s="33">
+        <v>5</v>
+      </c>
+      <c r="H16" s="33">
+        <v>0</v>
+      </c>
+      <c r="I16" s="33">
+        <v>0</v>
+      </c>
+      <c r="J16" s="33">
+        <v>43</v>
+      </c>
+      <c r="K16" s="33">
+        <v>50</v>
+      </c>
+      <c r="L16" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="B17" s="33">
+        <v>11</v>
+      </c>
+      <c r="C17" s="33">
+        <v>0</v>
+      </c>
+      <c r="D17" s="33">
+        <v>0</v>
+      </c>
+      <c r="E17" s="33">
+        <v>0</v>
+      </c>
+      <c r="F17" s="33">
+        <v>0</v>
+      </c>
+      <c r="G17" s="33">
+        <v>0</v>
+      </c>
+      <c r="H17" s="33">
+        <v>0</v>
+      </c>
+      <c r="I17" s="33">
+        <v>0</v>
+      </c>
+      <c r="J17" s="33">
+        <v>39</v>
+      </c>
+      <c r="K17" s="33">
+        <v>50</v>
+      </c>
+      <c r="L17" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
+        <v>206</v>
+      </c>
+      <c r="B18" s="33">
+        <v>10</v>
+      </c>
+      <c r="C18" s="33">
+        <v>0</v>
+      </c>
+      <c r="D18" s="33">
+        <v>0</v>
+      </c>
+      <c r="E18" s="33">
+        <v>0</v>
+      </c>
+      <c r="F18" s="33">
+        <v>0</v>
+      </c>
+      <c r="G18" s="33">
+        <v>4</v>
+      </c>
+      <c r="H18" s="33">
+        <v>0</v>
+      </c>
+      <c r="I18" s="33">
+        <v>0</v>
+      </c>
+      <c r="J18" s="33">
+        <v>40</v>
+      </c>
+      <c r="K18" s="33">
+        <v>50</v>
+      </c>
+      <c r="L18" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="B19" s="33">
+        <v>32</v>
+      </c>
+      <c r="C19" s="33">
+        <v>1</v>
+      </c>
+      <c r="D19" s="33">
+        <v>0</v>
+      </c>
+      <c r="E19" s="33">
+        <v>0</v>
+      </c>
+      <c r="F19" s="33">
+        <v>1</v>
+      </c>
+      <c r="G19" s="33">
+        <v>2</v>
+      </c>
+      <c r="H19" s="33">
+        <v>0</v>
+      </c>
+      <c r="I19" s="33">
+        <v>0</v>
+      </c>
+      <c r="J19" s="33">
+        <v>37</v>
+      </c>
+      <c r="K19" s="33">
+        <v>69</v>
+      </c>
+      <c r="L19" s="33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="B20" s="33">
+        <v>3</v>
+      </c>
+      <c r="C20" s="33">
+        <v>0</v>
+      </c>
+      <c r="D20" s="33">
+        <v>0</v>
+      </c>
+      <c r="E20" s="33">
+        <v>0</v>
+      </c>
+      <c r="F20" s="33">
+        <v>0</v>
+      </c>
+      <c r="G20" s="33">
+        <v>4</v>
+      </c>
+      <c r="H20" s="33">
+        <v>0</v>
+      </c>
+      <c r="I20" s="33">
+        <v>0</v>
+      </c>
+      <c r="J20" s="33">
+        <v>47</v>
+      </c>
+      <c r="K20" s="33">
+        <v>50</v>
+      </c>
+      <c r="L20" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="B21" s="33">
+        <v>10</v>
+      </c>
+      <c r="C21" s="33">
+        <v>0</v>
+      </c>
+      <c r="D21" s="33">
+        <v>0</v>
+      </c>
+      <c r="E21" s="33">
+        <v>0</v>
+      </c>
+      <c r="F21" s="33">
+        <v>0</v>
+      </c>
+      <c r="G21" s="33">
+        <v>3</v>
+      </c>
+      <c r="H21" s="33">
+        <v>0</v>
+      </c>
+      <c r="I21" s="33">
+        <v>0</v>
+      </c>
+      <c r="J21" s="33">
+        <v>40</v>
+      </c>
+      <c r="K21" s="33">
+        <v>50</v>
+      </c>
+      <c r="L21" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="B22" s="33">
+        <v>7</v>
+      </c>
+      <c r="C22" s="33">
+        <v>0</v>
+      </c>
+      <c r="D22" s="33">
+        <v>0</v>
+      </c>
+      <c r="E22" s="33">
+        <v>0</v>
+      </c>
+      <c r="F22" s="33">
+        <v>0</v>
+      </c>
+      <c r="G22" s="33">
+        <v>3</v>
+      </c>
+      <c r="H22" s="33">
+        <v>0</v>
+      </c>
+      <c r="I22" s="33">
+        <v>0</v>
+      </c>
+      <c r="J22" s="33">
+        <v>43</v>
+      </c>
+      <c r="K22" s="33">
+        <v>50</v>
+      </c>
+      <c r="L22" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
+        <v>211</v>
+      </c>
+      <c r="B23" s="33">
+        <v>4</v>
+      </c>
+      <c r="C23" s="33">
+        <v>0</v>
+      </c>
+      <c r="D23" s="33">
+        <v>0</v>
+      </c>
+      <c r="E23" s="33">
+        <v>0</v>
+      </c>
+      <c r="F23" s="33">
+        <v>0</v>
+      </c>
+      <c r="G23" s="33">
+        <v>4</v>
+      </c>
+      <c r="H23" s="33">
+        <v>0</v>
+      </c>
+      <c r="I23" s="33">
+        <v>0</v>
+      </c>
+      <c r="J23" s="33">
+        <v>46</v>
+      </c>
+      <c r="K23" s="33">
+        <v>50</v>
+      </c>
+      <c r="L23" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="B24" s="33">
+        <v>9</v>
+      </c>
+      <c r="C24" s="33">
+        <v>0</v>
+      </c>
+      <c r="D24" s="33">
+        <v>0</v>
+      </c>
+      <c r="E24" s="33">
+        <v>0</v>
+      </c>
+      <c r="F24" s="33">
+        <v>0</v>
+      </c>
+      <c r="G24" s="33">
+        <v>5</v>
+      </c>
+      <c r="H24" s="33">
+        <v>0</v>
+      </c>
+      <c r="I24" s="33">
+        <v>0</v>
+      </c>
+      <c r="J24" s="33">
+        <v>41</v>
+      </c>
+      <c r="K24" s="33">
+        <v>50</v>
+      </c>
+      <c r="L24" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="B25" s="33">
+        <v>2</v>
+      </c>
+      <c r="C25" s="33">
+        <v>0</v>
+      </c>
+      <c r="D25" s="33">
+        <v>0</v>
+      </c>
+      <c r="E25" s="33">
+        <v>0</v>
+      </c>
+      <c r="F25" s="33">
+        <v>0</v>
+      </c>
+      <c r="G25" s="33">
+        <v>8</v>
+      </c>
+      <c r="H25" s="33">
+        <v>0</v>
+      </c>
+      <c r="I25" s="33">
+        <v>0</v>
+      </c>
+      <c r="J25" s="33">
+        <v>48</v>
+      </c>
+      <c r="K25" s="33">
+        <v>50</v>
+      </c>
+      <c r="L25" s="33">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="33" t="s">
+        <v>214</v>
+      </c>
+      <c r="B26" s="33">
+        <v>6</v>
+      </c>
+      <c r="C26" s="33">
+        <v>0</v>
+      </c>
+      <c r="D26" s="33">
+        <v>0</v>
+      </c>
+      <c r="E26" s="33">
+        <v>0</v>
+      </c>
+      <c r="F26" s="33">
+        <v>0</v>
+      </c>
+      <c r="G26" s="33">
+        <v>3</v>
+      </c>
+      <c r="H26" s="33">
+        <v>0</v>
+      </c>
+      <c r="I26" s="33">
+        <v>0</v>
+      </c>
+      <c r="J26" s="33">
+        <v>44</v>
+      </c>
+      <c r="K26" s="33">
+        <v>50</v>
+      </c>
+      <c r="L26" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="B27" s="33">
+        <v>9</v>
+      </c>
+      <c r="C27" s="33">
+        <v>0</v>
+      </c>
+      <c r="D27" s="33">
+        <v>0</v>
+      </c>
+      <c r="E27" s="33">
+        <v>0</v>
+      </c>
+      <c r="F27" s="33">
+        <v>0</v>
+      </c>
+      <c r="G27" s="33">
+        <v>1</v>
+      </c>
+      <c r="H27" s="33">
+        <v>0</v>
+      </c>
+      <c r="I27" s="33">
+        <v>0</v>
+      </c>
+      <c r="J27" s="33">
+        <v>41</v>
+      </c>
+      <c r="K27" s="33">
+        <v>50</v>
+      </c>
+      <c r="L27" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="B28" s="33">
+        <v>8</v>
+      </c>
+      <c r="C28" s="33">
+        <v>1</v>
+      </c>
+      <c r="D28" s="33">
+        <v>0</v>
+      </c>
+      <c r="E28" s="33">
+        <v>0</v>
+      </c>
+      <c r="F28" s="33">
+        <v>1</v>
+      </c>
+      <c r="G28" s="33">
+        <v>3</v>
+      </c>
+      <c r="H28" s="33">
+        <v>0</v>
+      </c>
+      <c r="I28" s="33">
+        <v>0</v>
+      </c>
+      <c r="J28" s="33">
+        <v>34</v>
+      </c>
+      <c r="K28" s="33">
+        <v>42</v>
+      </c>
+      <c r="L28" s="33">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="B29" s="33">
+        <v>6</v>
+      </c>
+      <c r="C29" s="33">
+        <v>0</v>
+      </c>
+      <c r="D29" s="33">
+        <v>0</v>
+      </c>
+      <c r="E29" s="33">
+        <v>0</v>
+      </c>
+      <c r="F29" s="33">
+        <v>0</v>
+      </c>
+      <c r="G29" s="33">
+        <v>2</v>
+      </c>
+      <c r="H29" s="33">
+        <v>0</v>
+      </c>
+      <c r="I29" s="33">
+        <v>0</v>
+      </c>
+      <c r="J29" s="33">
+        <v>44</v>
+      </c>
+      <c r="K29" s="33">
+        <v>50</v>
+      </c>
+      <c r="L29" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="B30" s="33">
+        <v>6</v>
+      </c>
+      <c r="C30" s="33">
+        <v>0</v>
+      </c>
+      <c r="D30" s="33">
+        <v>1</v>
+      </c>
+      <c r="E30" s="33">
+        <v>0</v>
+      </c>
+      <c r="F30" s="33">
+        <v>0</v>
+      </c>
+      <c r="G30" s="33">
+        <v>1</v>
+      </c>
+      <c r="H30" s="33">
+        <v>0</v>
+      </c>
+      <c r="I30" s="33">
+        <v>0</v>
+      </c>
+      <c r="J30" s="33">
+        <v>43</v>
+      </c>
+      <c r="K30" s="33">
+        <v>50</v>
+      </c>
+      <c r="L30" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="B31" s="33">
+        <v>3</v>
+      </c>
+      <c r="C31" s="33">
+        <v>0</v>
+      </c>
+      <c r="D31" s="33">
+        <v>4</v>
+      </c>
+      <c r="E31" s="33">
+        <v>0</v>
+      </c>
+      <c r="F31" s="33">
+        <v>0</v>
+      </c>
+      <c r="G31" s="33">
+        <v>6</v>
+      </c>
+      <c r="H31" s="33">
+        <v>0</v>
+      </c>
+      <c r="I31" s="33">
+        <v>0</v>
+      </c>
+      <c r="J31" s="33">
+        <v>43</v>
+      </c>
+      <c r="K31" s="33">
+        <v>50</v>
+      </c>
+      <c r="L31" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="B32" s="33">
+        <v>6</v>
+      </c>
+      <c r="C32" s="33">
+        <v>0</v>
+      </c>
+      <c r="D32" s="33">
+        <v>1</v>
+      </c>
+      <c r="E32" s="33">
+        <v>0</v>
+      </c>
+      <c r="F32" s="33">
+        <v>1</v>
+      </c>
+      <c r="G32" s="33">
+        <v>9</v>
+      </c>
+      <c r="H32" s="33">
+        <v>0</v>
+      </c>
+      <c r="I32" s="33">
+        <v>0</v>
+      </c>
+      <c r="J32" s="33">
+        <v>60</v>
+      </c>
+      <c r="K32" s="33">
+        <v>68</v>
+      </c>
+      <c r="L32" s="33">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="B33" s="33">
+        <v>3</v>
+      </c>
+      <c r="C33" s="33">
+        <v>0</v>
+      </c>
+      <c r="D33" s="33">
+        <v>1</v>
+      </c>
+      <c r="E33" s="33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="33">
+        <v>0</v>
+      </c>
+      <c r="G33" s="33">
+        <v>3</v>
+      </c>
+      <c r="H33" s="33">
+        <v>0</v>
+      </c>
+      <c r="I33" s="33">
+        <v>1</v>
+      </c>
+      <c r="J33" s="33">
+        <v>46</v>
+      </c>
+      <c r="K33" s="33">
+        <v>50</v>
+      </c>
+      <c r="L33" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="B34" s="33">
+        <v>2</v>
+      </c>
+      <c r="C34" s="33">
+        <v>0</v>
+      </c>
+      <c r="D34" s="33">
+        <v>0</v>
+      </c>
+      <c r="E34" s="33">
+        <v>0</v>
+      </c>
+      <c r="F34" s="33">
+        <v>0</v>
+      </c>
+      <c r="G34" s="33">
+        <v>1</v>
+      </c>
+      <c r="H34" s="33">
+        <v>0</v>
+      </c>
+      <c r="I34" s="33">
+        <v>0</v>
+      </c>
+      <c r="J34" s="33">
+        <v>48</v>
+      </c>
+      <c r="K34" s="33">
+        <v>50</v>
+      </c>
+      <c r="L34" s="33">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="B35" s="33">
+        <v>6</v>
+      </c>
+      <c r="C35" s="33">
+        <v>0</v>
+      </c>
+      <c r="D35" s="33">
+        <v>1</v>
+      </c>
+      <c r="E35" s="33">
+        <v>0</v>
+      </c>
+      <c r="F35" s="33">
+        <v>0</v>
+      </c>
+      <c r="G35" s="33">
+        <v>5</v>
+      </c>
+      <c r="H35" s="33">
+        <v>0</v>
+      </c>
+      <c r="I35" s="33">
+        <v>1</v>
+      </c>
+      <c r="J35" s="33">
+        <v>43</v>
+      </c>
+      <c r="K35" s="33">
+        <v>50</v>
+      </c>
+      <c r="L35" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="B36" s="33">
+        <v>6</v>
+      </c>
+      <c r="C36" s="33">
+        <v>0</v>
+      </c>
+      <c r="D36" s="33">
+        <v>0</v>
+      </c>
+      <c r="E36" s="33">
+        <v>0</v>
+      </c>
+      <c r="F36" s="33">
+        <v>1</v>
+      </c>
+      <c r="G36" s="33">
+        <v>3</v>
+      </c>
+      <c r="H36" s="33">
+        <v>0</v>
+      </c>
+      <c r="I36" s="33">
+        <v>0</v>
+      </c>
+      <c r="J36" s="33">
+        <v>53</v>
+      </c>
+      <c r="K36" s="33">
+        <v>60</v>
+      </c>
+      <c r="L36" s="33">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="B37" s="33">
+        <v>17</v>
+      </c>
+      <c r="C37" s="33">
+        <v>0</v>
+      </c>
+      <c r="D37" s="33">
+        <v>0</v>
+      </c>
+      <c r="E37" s="33">
+        <v>0</v>
+      </c>
+      <c r="F37" s="33">
+        <v>0</v>
+      </c>
+      <c r="G37" s="33">
+        <v>7</v>
+      </c>
+      <c r="H37" s="33">
+        <v>0</v>
+      </c>
+      <c r="I37" s="33">
+        <v>0</v>
+      </c>
+      <c r="J37" s="33">
+        <v>33</v>
+      </c>
+      <c r="K37" s="33">
+        <v>50</v>
+      </c>
+      <c r="L37" s="33">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="B38" s="33">
+        <v>10</v>
+      </c>
+      <c r="C38" s="33">
+        <v>0</v>
+      </c>
+      <c r="D38" s="33">
+        <v>1</v>
+      </c>
+      <c r="E38" s="33">
+        <v>0</v>
+      </c>
+      <c r="F38" s="33">
+        <v>0</v>
+      </c>
+      <c r="G38" s="33">
+        <v>5</v>
+      </c>
+      <c r="H38" s="33">
+        <v>0</v>
+      </c>
+      <c r="I38" s="33">
+        <v>0</v>
+      </c>
+      <c r="J38" s="33">
+        <v>39</v>
+      </c>
+      <c r="K38" s="33">
+        <v>50</v>
+      </c>
+      <c r="L38" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="B39" s="33">
+        <v>11</v>
+      </c>
+      <c r="C39" s="33">
+        <v>0</v>
+      </c>
+      <c r="D39" s="33">
+        <v>1</v>
+      </c>
+      <c r="E39" s="33">
+        <v>0</v>
+      </c>
+      <c r="F39" s="33">
+        <v>0</v>
+      </c>
+      <c r="G39" s="33">
+        <v>3</v>
+      </c>
+      <c r="H39" s="33">
+        <v>0</v>
+      </c>
+      <c r="I39" s="33">
+        <v>0</v>
+      </c>
+      <c r="J39" s="33">
+        <v>38</v>
+      </c>
+      <c r="K39" s="33">
+        <v>50</v>
+      </c>
+      <c r="L39" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
+        <v>228</v>
+      </c>
+      <c r="B40" s="33">
+        <v>10</v>
+      </c>
+      <c r="C40" s="33">
+        <v>0</v>
+      </c>
+      <c r="D40" s="33">
+        <v>0</v>
+      </c>
+      <c r="E40" s="33">
+        <v>0</v>
+      </c>
+      <c r="F40" s="33">
+        <v>0</v>
+      </c>
+      <c r="G40" s="33">
+        <v>6</v>
+      </c>
+      <c r="H40" s="33">
+        <v>0</v>
+      </c>
+      <c r="I40" s="33">
+        <v>0</v>
+      </c>
+      <c r="J40" s="33">
+        <v>40</v>
+      </c>
+      <c r="K40" s="33">
+        <v>50</v>
+      </c>
+      <c r="L40" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="33" t="s">
+        <v>229</v>
+      </c>
+      <c r="B41" s="33">
+        <v>5</v>
+      </c>
+      <c r="C41" s="33">
+        <v>0</v>
+      </c>
+      <c r="D41" s="33">
+        <v>0</v>
+      </c>
+      <c r="E41" s="33">
+        <v>0</v>
+      </c>
+      <c r="F41" s="33">
+        <v>1</v>
+      </c>
+      <c r="G41" s="33">
+        <v>4</v>
+      </c>
+      <c r="H41" s="33">
+        <v>0</v>
+      </c>
+      <c r="I41" s="33">
+        <v>0</v>
+      </c>
+      <c r="J41" s="33">
+        <v>62</v>
+      </c>
+      <c r="K41" s="33">
+        <v>68</v>
+      </c>
+      <c r="L41" s="33">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="B42" s="33">
+        <v>11</v>
+      </c>
+      <c r="C42" s="33">
+        <v>0</v>
+      </c>
+      <c r="D42" s="33">
+        <v>2</v>
+      </c>
+      <c r="E42" s="33">
+        <v>0</v>
+      </c>
+      <c r="F42" s="33">
+        <v>0</v>
+      </c>
+      <c r="G42" s="33">
+        <v>0</v>
+      </c>
+      <c r="H42" s="33">
+        <v>0</v>
+      </c>
+      <c r="I42" s="33">
+        <v>0</v>
+      </c>
+      <c r="J42" s="33">
+        <v>37</v>
+      </c>
+      <c r="K42" s="33">
+        <v>50</v>
+      </c>
+      <c r="L42" s="33">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="s">
+        <v>231</v>
+      </c>
+      <c r="B43" s="33">
+        <v>11</v>
+      </c>
+      <c r="C43" s="33">
+        <v>0</v>
+      </c>
+      <c r="D43" s="33">
+        <v>0</v>
+      </c>
+      <c r="E43" s="33">
+        <v>0</v>
+      </c>
+      <c r="F43" s="33">
+        <v>0</v>
+      </c>
+      <c r="G43" s="33">
+        <v>3</v>
+      </c>
+      <c r="H43" s="33">
+        <v>0</v>
+      </c>
+      <c r="I43" s="33">
+        <v>0</v>
+      </c>
+      <c r="J43" s="33">
+        <v>39</v>
+      </c>
+      <c r="K43" s="33">
+        <v>50</v>
+      </c>
+      <c r="L43" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="B44" s="33">
+        <v>7</v>
+      </c>
+      <c r="C44" s="33">
+        <v>0</v>
+      </c>
+      <c r="D44" s="33">
+        <v>1</v>
+      </c>
+      <c r="E44" s="33">
+        <v>0</v>
+      </c>
+      <c r="F44" s="33">
+        <v>0</v>
+      </c>
+      <c r="G44" s="33">
+        <v>4</v>
+      </c>
+      <c r="H44" s="33">
+        <v>0</v>
+      </c>
+      <c r="I44" s="33">
+        <v>0</v>
+      </c>
+      <c r="J44" s="33">
+        <v>42</v>
+      </c>
+      <c r="K44" s="33">
+        <v>50</v>
+      </c>
+      <c r="L44" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="B45" s="33">
+        <v>6</v>
+      </c>
+      <c r="C45" s="33">
+        <v>0</v>
+      </c>
+      <c r="D45" s="33">
+        <v>0</v>
+      </c>
+      <c r="E45" s="33">
+        <v>0</v>
+      </c>
+      <c r="F45" s="33">
+        <v>1</v>
+      </c>
+      <c r="G45" s="33">
+        <v>3</v>
+      </c>
+      <c r="H45" s="33">
+        <v>0</v>
+      </c>
+      <c r="I45" s="33">
+        <v>0</v>
+      </c>
+      <c r="J45" s="33">
+        <v>30</v>
+      </c>
+      <c r="K45" s="33">
+        <v>37</v>
+      </c>
+      <c r="L45" s="33">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="B46" s="33">
+        <v>9</v>
+      </c>
+      <c r="C46" s="33">
+        <v>0</v>
+      </c>
+      <c r="D46" s="33">
+        <v>0</v>
+      </c>
+      <c r="E46" s="33">
+        <v>0</v>
+      </c>
+      <c r="F46" s="33">
+        <v>0</v>
+      </c>
+      <c r="G46" s="33">
+        <v>5</v>
+      </c>
+      <c r="H46" s="33">
+        <v>0</v>
+      </c>
+      <c r="I46" s="33">
+        <v>0</v>
+      </c>
+      <c r="J46" s="33">
+        <v>41</v>
+      </c>
+      <c r="K46" s="33">
+        <v>50</v>
+      </c>
+      <c r="L46" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="33" t="s">
+        <v>235</v>
+      </c>
+      <c r="B47" s="33">
+        <v>4</v>
+      </c>
+      <c r="C47" s="33">
+        <v>0</v>
+      </c>
+      <c r="D47" s="33">
+        <v>0</v>
+      </c>
+      <c r="E47" s="33">
+        <v>0</v>
+      </c>
+      <c r="F47" s="33">
+        <v>0</v>
+      </c>
+      <c r="G47" s="33">
+        <v>3</v>
+      </c>
+      <c r="H47" s="33">
+        <v>0</v>
+      </c>
+      <c r="I47" s="33">
+        <v>0</v>
+      </c>
+      <c r="J47" s="33">
+        <v>46</v>
+      </c>
+      <c r="K47" s="33">
+        <v>50</v>
+      </c>
+      <c r="L47" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="33" t="s">
+        <v>236</v>
+      </c>
+      <c r="B48" s="33">
+        <v>3</v>
+      </c>
+      <c r="C48" s="33">
+        <v>0</v>
+      </c>
+      <c r="D48" s="33">
+        <v>2</v>
+      </c>
+      <c r="E48" s="33">
+        <v>0</v>
+      </c>
+      <c r="F48" s="33">
+        <v>0</v>
+      </c>
+      <c r="G48" s="33">
+        <v>2</v>
+      </c>
+      <c r="H48" s="33">
+        <v>0</v>
+      </c>
+      <c r="I48" s="33">
+        <v>0</v>
+      </c>
+      <c r="J48" s="33">
+        <v>45</v>
+      </c>
+      <c r="K48" s="33">
+        <v>50</v>
+      </c>
+      <c r="L48" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="B49" s="33">
+        <v>6</v>
+      </c>
+      <c r="C49" s="33">
+        <v>0</v>
+      </c>
+      <c r="D49" s="33">
+        <v>2</v>
+      </c>
+      <c r="E49" s="33">
+        <v>0</v>
+      </c>
+      <c r="F49" s="33">
+        <v>0</v>
+      </c>
+      <c r="G49" s="33">
+        <v>3</v>
+      </c>
+      <c r="H49" s="33">
+        <v>0</v>
+      </c>
+      <c r="I49" s="33">
+        <v>0</v>
+      </c>
+      <c r="J49" s="33">
+        <v>42</v>
+      </c>
+      <c r="K49" s="33">
+        <v>50</v>
+      </c>
+      <c r="L49" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="s">
+        <v>238</v>
+      </c>
+      <c r="B50" s="33">
+        <v>3</v>
+      </c>
+      <c r="C50" s="33">
+        <v>0</v>
+      </c>
+      <c r="D50" s="33">
+        <v>2</v>
+      </c>
+      <c r="E50" s="33">
+        <v>0</v>
+      </c>
+      <c r="F50" s="33">
+        <v>0</v>
+      </c>
+      <c r="G50" s="33">
+        <v>8</v>
+      </c>
+      <c r="H50" s="33">
+        <v>0</v>
+      </c>
+      <c r="I50" s="33">
+        <v>0</v>
+      </c>
+      <c r="J50" s="33">
+        <v>45</v>
+      </c>
+      <c r="K50" s="33">
+        <v>50</v>
+      </c>
+      <c r="L50" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="B51" s="33">
+        <v>9</v>
+      </c>
+      <c r="C51" s="33">
+        <v>1</v>
+      </c>
+      <c r="D51" s="33">
+        <v>3</v>
+      </c>
+      <c r="E51" s="33">
+        <v>0</v>
+      </c>
+      <c r="F51" s="33">
+        <v>1</v>
+      </c>
+      <c r="G51" s="33">
+        <v>4</v>
+      </c>
+      <c r="H51" s="33">
+        <v>0</v>
+      </c>
+      <c r="I51" s="33">
+        <v>0</v>
+      </c>
+      <c r="J51" s="33">
+        <v>34</v>
+      </c>
+      <c r="K51" s="33">
+        <v>46</v>
+      </c>
+      <c r="L51" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="B52" s="33">
+        <v>7</v>
+      </c>
+      <c r="C52" s="33">
+        <v>0</v>
+      </c>
+      <c r="D52" s="33">
+        <v>1</v>
+      </c>
+      <c r="E52" s="33">
+        <v>0</v>
+      </c>
+      <c r="F52" s="33">
+        <v>0</v>
+      </c>
+      <c r="G52" s="33">
+        <v>4</v>
+      </c>
+      <c r="H52" s="33">
+        <v>0</v>
+      </c>
+      <c r="I52" s="33">
+        <v>0</v>
+      </c>
+      <c r="J52" s="33">
+        <v>42</v>
+      </c>
+      <c r="K52" s="33">
+        <v>50</v>
+      </c>
+      <c r="L52" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="33" t="s">
+        <v>241</v>
+      </c>
+      <c r="B53" s="33">
+        <v>11</v>
+      </c>
+      <c r="C53" s="33">
+        <v>0</v>
+      </c>
+      <c r="D53" s="33">
+        <v>0</v>
+      </c>
+      <c r="E53" s="33">
+        <v>0</v>
+      </c>
+      <c r="F53" s="33">
+        <v>0</v>
+      </c>
+      <c r="G53" s="33">
+        <v>3</v>
+      </c>
+      <c r="H53" s="33">
+        <v>0</v>
+      </c>
+      <c r="I53" s="33">
+        <v>0</v>
+      </c>
+      <c r="J53" s="33">
+        <v>39</v>
+      </c>
+      <c r="K53" s="33">
+        <v>50</v>
+      </c>
+      <c r="L53" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="33" t="s">
+        <v>242</v>
+      </c>
+      <c r="B54" s="33">
+        <v>6</v>
+      </c>
+      <c r="C54" s="33">
+        <v>0</v>
+      </c>
+      <c r="D54" s="33">
+        <v>0</v>
+      </c>
+      <c r="E54" s="33">
+        <v>0</v>
+      </c>
+      <c r="F54" s="33">
+        <v>0</v>
+      </c>
+      <c r="G54" s="33">
+        <v>7</v>
+      </c>
+      <c r="H54" s="33">
+        <v>0</v>
+      </c>
+      <c r="I54" s="33">
+        <v>0</v>
+      </c>
+      <c r="J54" s="33">
+        <v>44</v>
+      </c>
+      <c r="K54" s="33">
+        <v>50</v>
+      </c>
+      <c r="L54" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="B55" s="33">
+        <v>9</v>
+      </c>
+      <c r="C55" s="33">
+        <v>0</v>
+      </c>
+      <c r="D55" s="33">
+        <v>0</v>
+      </c>
+      <c r="E55" s="33">
+        <v>0</v>
+      </c>
+      <c r="F55" s="33">
+        <v>0</v>
+      </c>
+      <c r="G55" s="33">
+        <v>5</v>
+      </c>
+      <c r="H55" s="33">
+        <v>0</v>
+      </c>
+      <c r="I55" s="33">
+        <v>0</v>
+      </c>
+      <c r="J55" s="33">
+        <v>41</v>
+      </c>
+      <c r="K55" s="33">
+        <v>50</v>
+      </c>
+      <c r="L55" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="B56" s="33">
+        <v>14</v>
+      </c>
+      <c r="C56" s="33">
+        <v>0</v>
+      </c>
+      <c r="D56" s="33">
+        <v>0</v>
+      </c>
+      <c r="E56" s="33">
+        <v>0</v>
+      </c>
+      <c r="F56" s="33">
+        <v>0</v>
+      </c>
+      <c r="G56" s="33">
+        <v>2</v>
+      </c>
+      <c r="H56" s="33">
+        <v>0</v>
+      </c>
+      <c r="I56" s="33">
+        <v>0</v>
+      </c>
+      <c r="J56" s="33">
+        <v>36</v>
+      </c>
+      <c r="K56" s="33">
+        <v>50</v>
+      </c>
+      <c r="L56" s="33">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="B57" s="33">
+        <v>8</v>
+      </c>
+      <c r="C57" s="33">
+        <v>1</v>
+      </c>
+      <c r="D57" s="33">
+        <v>0</v>
+      </c>
+      <c r="E57" s="33">
+        <v>0</v>
+      </c>
+      <c r="F57" s="33">
+        <v>1</v>
+      </c>
+      <c r="G57" s="33">
+        <v>6</v>
+      </c>
+      <c r="H57" s="33">
+        <v>0</v>
+      </c>
+      <c r="I57" s="33">
+        <v>0</v>
+      </c>
+      <c r="J57" s="33">
+        <v>37</v>
+      </c>
+      <c r="K57" s="33">
+        <v>45</v>
+      </c>
+      <c r="L57" s="33">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="33" t="s">
+        <v>246</v>
+      </c>
+      <c r="B58" s="33">
+        <v>5</v>
+      </c>
+      <c r="C58" s="33">
+        <v>0</v>
+      </c>
+      <c r="D58" s="33">
+        <v>0</v>
+      </c>
+      <c r="E58" s="33">
+        <v>0</v>
+      </c>
+      <c r="F58" s="33">
+        <v>0</v>
+      </c>
+      <c r="G58" s="33">
+        <v>3</v>
+      </c>
+      <c r="H58" s="33">
+        <v>0</v>
+      </c>
+      <c r="I58" s="33">
+        <v>0</v>
+      </c>
+      <c r="J58" s="33">
+        <v>45</v>
+      </c>
+      <c r="K58" s="33">
+        <v>50</v>
+      </c>
+      <c r="L58" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="B59" s="33">
+        <v>12</v>
+      </c>
+      <c r="C59" s="33">
+        <v>0</v>
+      </c>
+      <c r="D59" s="33">
+        <v>0</v>
+      </c>
+      <c r="E59" s="33">
+        <v>0</v>
+      </c>
+      <c r="F59" s="33">
+        <v>0</v>
+      </c>
+      <c r="G59" s="33">
+        <v>1</v>
+      </c>
+      <c r="H59" s="33">
+        <v>0</v>
+      </c>
+      <c r="I59" s="33">
+        <v>0</v>
+      </c>
+      <c r="J59" s="33">
+        <v>38</v>
+      </c>
+      <c r="K59" s="33">
+        <v>50</v>
+      </c>
+      <c r="L59" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="B60" s="33">
+        <v>9</v>
+      </c>
+      <c r="C60" s="33">
+        <v>0</v>
+      </c>
+      <c r="D60" s="33">
+        <v>2</v>
+      </c>
+      <c r="E60" s="33">
+        <v>0</v>
+      </c>
+      <c r="F60" s="33">
+        <v>0</v>
+      </c>
+      <c r="G60" s="33">
+        <v>2</v>
+      </c>
+      <c r="H60" s="33">
+        <v>0</v>
+      </c>
+      <c r="I60" s="33">
+        <v>0</v>
+      </c>
+      <c r="J60" s="33">
+        <v>39</v>
+      </c>
+      <c r="K60" s="33">
+        <v>50</v>
+      </c>
+      <c r="L60" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="B61" s="33">
+        <v>7</v>
+      </c>
+      <c r="C61" s="33">
+        <v>0</v>
+      </c>
+      <c r="D61" s="33">
+        <v>0</v>
+      </c>
+      <c r="E61" s="33">
+        <v>0</v>
+      </c>
+      <c r="F61" s="33">
+        <v>0</v>
+      </c>
+      <c r="G61" s="33">
+        <v>6</v>
+      </c>
+      <c r="H61" s="33">
+        <v>0</v>
+      </c>
+      <c r="I61" s="33">
+        <v>0</v>
+      </c>
+      <c r="J61" s="33">
+        <v>43</v>
+      </c>
+      <c r="K61" s="33">
+        <v>50</v>
+      </c>
+      <c r="L61" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="33" t="s">
+        <v>250</v>
+      </c>
+      <c r="B62" s="33">
+        <v>8</v>
+      </c>
+      <c r="C62" s="33">
+        <v>0</v>
+      </c>
+      <c r="D62" s="33">
+        <v>0</v>
+      </c>
+      <c r="E62" s="33">
+        <v>0</v>
+      </c>
+      <c r="F62" s="33">
+        <v>0</v>
+      </c>
+      <c r="G62" s="33">
+        <v>4</v>
+      </c>
+      <c r="H62" s="33">
+        <v>0</v>
+      </c>
+      <c r="I62" s="33">
+        <v>0</v>
+      </c>
+      <c r="J62" s="33">
+        <v>42</v>
+      </c>
+      <c r="K62" s="33">
+        <v>50</v>
+      </c>
+      <c r="L62" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="B63" s="33">
+        <v>13</v>
+      </c>
+      <c r="C63" s="33">
+        <v>0</v>
+      </c>
+      <c r="D63" s="33">
+        <v>0</v>
+      </c>
+      <c r="E63" s="33">
+        <v>0</v>
+      </c>
+      <c r="F63" s="33">
+        <v>1</v>
+      </c>
+      <c r="G63" s="33">
+        <v>1</v>
+      </c>
+      <c r="H63" s="33">
+        <v>0</v>
+      </c>
+      <c r="I63" s="33">
+        <v>0</v>
+      </c>
+      <c r="J63" s="33">
+        <v>42</v>
+      </c>
+      <c r="K63" s="33">
+        <v>56</v>
+      </c>
+      <c r="L63" s="33">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="34" t="s">
+        <v>252</v>
+      </c>
+      <c r="B64" s="36">
+        <f>SUM(B2:B63)</f>
+        <v>494</v>
+      </c>
+      <c r="C64" s="36">
+        <f>SUM(C2:C63)</f>
+        <v>4</v>
+      </c>
+      <c r="D64" s="36">
+        <f>SUM(D2:D63)</f>
+        <v>30</v>
+      </c>
+      <c r="E64" s="36">
+        <f>SUM(E2:E63)</f>
+        <v>0</v>
+      </c>
+      <c r="F64" s="36">
+        <f>SUM(F2:F63)</f>
+        <v>11</v>
+      </c>
+      <c r="G64" s="36">
+        <f>SUM(G2:G63)</f>
+        <v>229</v>
+      </c>
+      <c r="H64" s="36">
+        <f>SUM(H2:H63)</f>
+        <v>0</v>
+      </c>
+      <c r="I64" s="34">
+        <f>SUM(I2:I63)</f>
+        <v>2</v>
+      </c>
+      <c r="J64" s="36">
+        <f>SUM(J2:J63)</f>
+        <v>2624</v>
+      </c>
+      <c r="K64" s="36">
+        <f>SUM(K2:K63)</f>
+        <v>3155</v>
+      </c>
+      <c r="L64" s="36">
+        <f>SUM(L2:L63)</f>
+        <v>3675</v>
+      </c>
+    </row>
+    <row r="65" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>39</v>
+      </c>
+      <c r="F65">
+        <f>G64</f>
+        <v>229</v>
+      </c>
+      <c r="J65">
+        <f>B64-C64</f>
+        <v>490</v>
+      </c>
+    </row>
+    <row r="66" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>40</v>
+      </c>
+      <c r="F66">
+        <f>B64</f>
+        <v>494</v>
+      </c>
+      <c r="J66">
+        <f>D64-E64</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="67" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
+        <v>41</v>
+      </c>
+      <c r="F67">
+        <v>25</v>
+      </c>
+      <c r="J67">
+        <f>F73</f>
+        <v>3155</v>
+      </c>
+    </row>
+    <row r="68" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>42</v>
+      </c>
+      <c r="F68">
+        <v>5</v>
+      </c>
+      <c r="J68" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="69" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F69" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="J69">
+        <f>SUM(J65:J68)</f>
+        <v>3675</v>
+      </c>
+    </row>
+    <row r="70" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <f>SUM(F65:F69)</f>
+        <v>753</v>
+      </c>
+      <c r="J70" s="35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="71" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E71" t="s">
+        <v>45</v>
+      </c>
+      <c r="F71">
+        <f>K64-F70</f>
+        <v>2402</v>
+      </c>
+      <c r="J71">
+        <f>J69-L64</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F72" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="73" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <f>F71+F70</f>
+        <v>3155</v>
+      </c>
+    </row>
+    <row r="74" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <f>F73-K64</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:K31"/>
   <sheetViews>

</xml_diff>

<commit_message>
nmv 06 12 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 6.1 TO 6.6.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 6.1 TO 6.6.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9EDA1D-39EA-4B26-9598-BCD11375EBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02AD10D-1A12-4E3D-BD58-77129137A504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="6.1" sheetId="15" r:id="rId1"/>
     <sheet name="6.2" sheetId="16" r:id="rId2"/>
     <sheet name="6.3" sheetId="17" r:id="rId3"/>
-    <sheet name="total 6.1 to 6.6" sheetId="7" r:id="rId4"/>
+    <sheet name="6.4" sheetId="18" r:id="rId4"/>
+    <sheet name="total 6.1 to 6.6" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="305">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -1993,6 +1994,162 @@
   <si>
     <t>62</t>
   </si>
+  <si>
+    <t>6.4.1.1 :</t>
+  </si>
+  <si>
+    <t>6.4.1.2 :</t>
+  </si>
+  <si>
+    <t>6.4.1.3 :</t>
+  </si>
+  <si>
+    <t>6.4.1.4 :</t>
+  </si>
+  <si>
+    <t>6.4.1.5 :</t>
+  </si>
+  <si>
+    <t>6.4.2.1 :</t>
+  </si>
+  <si>
+    <t>6.4.2.2 :</t>
+  </si>
+  <si>
+    <t>6.4.2.3 :</t>
+  </si>
+  <si>
+    <t>6.4.2.4 :</t>
+  </si>
+  <si>
+    <t>6.4.2.5 :</t>
+  </si>
+  <si>
+    <t>6.4.2.6 :</t>
+  </si>
+  <si>
+    <t>6.4.3.1 :</t>
+  </si>
+  <si>
+    <t>6.4.3.2 :</t>
+  </si>
+  <si>
+    <t>6.4.3.3 :</t>
+  </si>
+  <si>
+    <t>6.4.3.4 :</t>
+  </si>
+  <si>
+    <t>6.4.4.1 :</t>
+  </si>
+  <si>
+    <t>6.4.4.2 :</t>
+  </si>
+  <si>
+    <t>6.4.4.3 :</t>
+  </si>
+  <si>
+    <t>6.4.4.4 :</t>
+  </si>
+  <si>
+    <t>6.4.5.1 :</t>
+  </si>
+  <si>
+    <t>6.4.5.2 :</t>
+  </si>
+  <si>
+    <t>6.4.5.3 :</t>
+  </si>
+  <si>
+    <t>6.4.5.4 :</t>
+  </si>
+  <si>
+    <t>6.4.5.5 :</t>
+  </si>
+  <si>
+    <t>6.4.5.6 :</t>
+  </si>
+  <si>
+    <t>6.4.5.7 :</t>
+  </si>
+  <si>
+    <t>6.4.6.1 :</t>
+  </si>
+  <si>
+    <t>6.4.6.2 :</t>
+  </si>
+  <si>
+    <t>6.4.6.3 :</t>
+  </si>
+  <si>
+    <t>6.4.6.4 :</t>
+  </si>
+  <si>
+    <t>6.4.7.1 :</t>
+  </si>
+  <si>
+    <t>6.4.7.2 :</t>
+  </si>
+  <si>
+    <t>6.4.7.3 :</t>
+  </si>
+  <si>
+    <t>6.4.8.1 :</t>
+  </si>
+  <si>
+    <t>6.4.8.2 :</t>
+  </si>
+  <si>
+    <t>6.4.8.3 :</t>
+  </si>
+  <si>
+    <t>6.4.9.1 :</t>
+  </si>
+  <si>
+    <t>6.4.9.2 :</t>
+  </si>
+  <si>
+    <t>6.4.9.3 :</t>
+  </si>
+  <si>
+    <t>6.4.9.4 :</t>
+  </si>
+  <si>
+    <t>6.4.9.5 :</t>
+  </si>
+  <si>
+    <t>6.4.10.1 :</t>
+  </si>
+  <si>
+    <t>6.4.10.2 :</t>
+  </si>
+  <si>
+    <t>6.4.10.3 :</t>
+  </si>
+  <si>
+    <t>6.4.10.4 :</t>
+  </si>
+  <si>
+    <t>6.4.10.5 :</t>
+  </si>
+  <si>
+    <t>6.4.10.6 :</t>
+  </si>
+  <si>
+    <t>6.4.11.1 :</t>
+  </si>
+  <si>
+    <t>6.4.11.2 :</t>
+  </si>
+  <si>
+    <t>6.4.11.3 :</t>
+  </si>
+  <si>
+    <t>6.4.11.4 :</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
 </sst>
 </file>
 
@@ -2188,7 +2345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2285,6 +2442,10 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8124,9 +8285,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02ADB140-5197-4869-A498-C69E75D5151E}">
   <dimension ref="A1:L74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:L64"/>
+      <selection pane="bottomLeft" activeCell="E65" sqref="E65:J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10542,47 +10703,47 @@
         <v>252</v>
       </c>
       <c r="B64" s="36">
-        <f>SUM(B2:B63)</f>
+        <f t="shared" ref="B64:L64" si="0">SUM(B2:B63)</f>
         <v>494</v>
       </c>
       <c r="C64" s="36">
-        <f>SUM(C2:C63)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D64" s="36">
-        <f>SUM(D2:D63)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="E64" s="36">
-        <f>SUM(E2:E63)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F64" s="36">
-        <f>SUM(F2:F63)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G64" s="36">
-        <f>SUM(G2:G63)</f>
+        <f t="shared" si="0"/>
         <v>229</v>
       </c>
       <c r="H64" s="36">
-        <f>SUM(H2:H63)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I64" s="34">
-        <f>SUM(I2:I63)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J64" s="36">
-        <f>SUM(J2:J63)</f>
+        <f t="shared" si="0"/>
         <v>2624</v>
       </c>
       <c r="K64" s="36">
-        <f>SUM(K2:K63)</f>
+        <f t="shared" si="0"/>
         <v>3155</v>
       </c>
       <c r="L64" s="36">
-        <f>SUM(L2:L63)</f>
+        <f t="shared" si="0"/>
         <v>3675</v>
       </c>
     </row>
@@ -10689,6 +10850,2162 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95756750-C929-4133-9B35-850FD96AC5E9}">
+  <dimension ref="A1:L63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L44" sqref="L44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="B2" s="33">
+        <v>18</v>
+      </c>
+      <c r="C2" s="33">
+        <v>0</v>
+      </c>
+      <c r="D2" s="33">
+        <v>0</v>
+      </c>
+      <c r="E2" s="33">
+        <v>0</v>
+      </c>
+      <c r="F2" s="33">
+        <v>0</v>
+      </c>
+      <c r="G2" s="33">
+        <v>3</v>
+      </c>
+      <c r="H2" s="33">
+        <v>0</v>
+      </c>
+      <c r="I2" s="33">
+        <v>0</v>
+      </c>
+      <c r="J2" s="33">
+        <v>32</v>
+      </c>
+      <c r="K2" s="33">
+        <v>50</v>
+      </c>
+      <c r="L2" s="33">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="B3" s="33">
+        <v>10</v>
+      </c>
+      <c r="C3" s="33">
+        <v>0</v>
+      </c>
+      <c r="D3" s="33">
+        <v>2</v>
+      </c>
+      <c r="E3" s="33">
+        <v>0</v>
+      </c>
+      <c r="F3" s="33">
+        <v>0</v>
+      </c>
+      <c r="G3" s="33">
+        <v>5</v>
+      </c>
+      <c r="H3" s="33">
+        <v>0</v>
+      </c>
+      <c r="I3" s="33">
+        <v>0</v>
+      </c>
+      <c r="J3" s="33">
+        <v>38</v>
+      </c>
+      <c r="K3" s="33">
+        <v>50</v>
+      </c>
+      <c r="L3" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="B4" s="33">
+        <v>8</v>
+      </c>
+      <c r="C4" s="33">
+        <v>0</v>
+      </c>
+      <c r="D4" s="33">
+        <v>1</v>
+      </c>
+      <c r="E4" s="33">
+        <v>0</v>
+      </c>
+      <c r="F4" s="33">
+        <v>0</v>
+      </c>
+      <c r="G4" s="33">
+        <v>2</v>
+      </c>
+      <c r="H4" s="33">
+        <v>0</v>
+      </c>
+      <c r="I4" s="33">
+        <v>0</v>
+      </c>
+      <c r="J4" s="33">
+        <v>41</v>
+      </c>
+      <c r="K4" s="33">
+        <v>50</v>
+      </c>
+      <c r="L4" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="B5" s="33">
+        <v>10</v>
+      </c>
+      <c r="C5" s="33">
+        <v>0</v>
+      </c>
+      <c r="D5" s="33">
+        <v>0</v>
+      </c>
+      <c r="E5" s="33">
+        <v>0</v>
+      </c>
+      <c r="F5" s="33">
+        <v>0</v>
+      </c>
+      <c r="G5" s="33">
+        <v>4</v>
+      </c>
+      <c r="H5" s="33">
+        <v>0</v>
+      </c>
+      <c r="I5" s="33">
+        <v>0</v>
+      </c>
+      <c r="J5" s="33">
+        <v>40</v>
+      </c>
+      <c r="K5" s="33">
+        <v>50</v>
+      </c>
+      <c r="L5" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>257</v>
+      </c>
+      <c r="B6" s="33">
+        <v>4</v>
+      </c>
+      <c r="C6" s="33">
+        <v>0</v>
+      </c>
+      <c r="D6" s="33">
+        <v>0</v>
+      </c>
+      <c r="E6" s="33">
+        <v>0</v>
+      </c>
+      <c r="F6" s="33">
+        <v>1</v>
+      </c>
+      <c r="G6" s="33">
+        <v>3</v>
+      </c>
+      <c r="H6" s="33">
+        <v>0</v>
+      </c>
+      <c r="I6" s="33">
+        <v>0</v>
+      </c>
+      <c r="J6" s="33">
+        <v>27</v>
+      </c>
+      <c r="K6" s="33">
+        <v>32</v>
+      </c>
+      <c r="L6" s="33">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="B7" s="33">
+        <v>7</v>
+      </c>
+      <c r="C7" s="33">
+        <v>0</v>
+      </c>
+      <c r="D7" s="33">
+        <v>0</v>
+      </c>
+      <c r="E7" s="33">
+        <v>0</v>
+      </c>
+      <c r="F7" s="33">
+        <v>0</v>
+      </c>
+      <c r="G7" s="33">
+        <v>5</v>
+      </c>
+      <c r="H7" s="33">
+        <v>0</v>
+      </c>
+      <c r="I7" s="33">
+        <v>0</v>
+      </c>
+      <c r="J7" s="33">
+        <v>43</v>
+      </c>
+      <c r="K7" s="33">
+        <v>50</v>
+      </c>
+      <c r="L7" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="B8" s="33">
+        <v>7</v>
+      </c>
+      <c r="C8" s="33">
+        <v>0</v>
+      </c>
+      <c r="D8" s="33">
+        <v>0</v>
+      </c>
+      <c r="E8" s="33">
+        <v>0</v>
+      </c>
+      <c r="F8" s="33">
+        <v>0</v>
+      </c>
+      <c r="G8" s="33">
+        <v>2</v>
+      </c>
+      <c r="H8" s="33">
+        <v>0</v>
+      </c>
+      <c r="I8" s="33">
+        <v>0</v>
+      </c>
+      <c r="J8" s="33">
+        <v>43</v>
+      </c>
+      <c r="K8" s="33">
+        <v>50</v>
+      </c>
+      <c r="L8" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="B9" s="33">
+        <v>4</v>
+      </c>
+      <c r="C9" s="33">
+        <v>0</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0</v>
+      </c>
+      <c r="E9" s="33">
+        <v>0</v>
+      </c>
+      <c r="F9" s="33">
+        <v>0</v>
+      </c>
+      <c r="G9" s="33">
+        <v>4</v>
+      </c>
+      <c r="H9" s="33">
+        <v>0</v>
+      </c>
+      <c r="I9" s="33">
+        <v>0</v>
+      </c>
+      <c r="J9" s="33">
+        <v>46</v>
+      </c>
+      <c r="K9" s="33">
+        <v>50</v>
+      </c>
+      <c r="L9" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="B10" s="33">
+        <v>4</v>
+      </c>
+      <c r="C10" s="33">
+        <v>0</v>
+      </c>
+      <c r="D10" s="33">
+        <v>0</v>
+      </c>
+      <c r="E10" s="33">
+        <v>0</v>
+      </c>
+      <c r="F10" s="33">
+        <v>0</v>
+      </c>
+      <c r="G10" s="33">
+        <v>2</v>
+      </c>
+      <c r="H10" s="33">
+        <v>0</v>
+      </c>
+      <c r="I10" s="33">
+        <v>0</v>
+      </c>
+      <c r="J10" s="33">
+        <v>46</v>
+      </c>
+      <c r="K10" s="33">
+        <v>50</v>
+      </c>
+      <c r="L10" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="B11" s="33">
+        <v>11</v>
+      </c>
+      <c r="C11" s="33">
+        <v>0</v>
+      </c>
+      <c r="D11" s="33">
+        <v>0</v>
+      </c>
+      <c r="E11" s="33">
+        <v>0</v>
+      </c>
+      <c r="F11" s="33">
+        <v>0</v>
+      </c>
+      <c r="G11" s="33">
+        <v>3</v>
+      </c>
+      <c r="H11" s="33">
+        <v>0</v>
+      </c>
+      <c r="I11" s="33">
+        <v>0</v>
+      </c>
+      <c r="J11" s="33">
+        <v>39</v>
+      </c>
+      <c r="K11" s="33">
+        <v>50</v>
+      </c>
+      <c r="L11" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="B12" s="33">
+        <v>14</v>
+      </c>
+      <c r="C12" s="33">
+        <v>1</v>
+      </c>
+      <c r="D12" s="33">
+        <v>0</v>
+      </c>
+      <c r="E12" s="33">
+        <v>0</v>
+      </c>
+      <c r="F12" s="33">
+        <v>1</v>
+      </c>
+      <c r="G12" s="33">
+        <v>8</v>
+      </c>
+      <c r="H12" s="33">
+        <v>0</v>
+      </c>
+      <c r="I12" s="33">
+        <v>0</v>
+      </c>
+      <c r="J12" s="33">
+        <v>62</v>
+      </c>
+      <c r="K12" s="33">
+        <v>76</v>
+      </c>
+      <c r="L12" s="33">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="B13" s="33">
+        <v>5</v>
+      </c>
+      <c r="C13" s="33">
+        <v>0</v>
+      </c>
+      <c r="D13" s="33">
+        <v>0</v>
+      </c>
+      <c r="E13" s="33">
+        <v>0</v>
+      </c>
+      <c r="F13" s="33">
+        <v>0</v>
+      </c>
+      <c r="G13" s="33">
+        <v>0</v>
+      </c>
+      <c r="H13" s="33">
+        <v>0</v>
+      </c>
+      <c r="I13" s="33">
+        <v>0</v>
+      </c>
+      <c r="J13" s="33">
+        <v>45</v>
+      </c>
+      <c r="K13" s="33">
+        <v>50</v>
+      </c>
+      <c r="L13" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>265</v>
+      </c>
+      <c r="B14" s="33">
+        <v>13</v>
+      </c>
+      <c r="C14" s="33">
+        <v>0</v>
+      </c>
+      <c r="D14" s="33">
+        <v>0</v>
+      </c>
+      <c r="E14" s="33">
+        <v>0</v>
+      </c>
+      <c r="F14" s="33">
+        <v>0</v>
+      </c>
+      <c r="G14" s="33">
+        <v>6</v>
+      </c>
+      <c r="H14" s="33">
+        <v>0</v>
+      </c>
+      <c r="I14" s="33">
+        <v>0</v>
+      </c>
+      <c r="J14" s="33">
+        <v>37</v>
+      </c>
+      <c r="K14" s="33">
+        <v>50</v>
+      </c>
+      <c r="L14" s="33">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>266</v>
+      </c>
+      <c r="B15" s="33">
+        <v>9</v>
+      </c>
+      <c r="C15" s="33">
+        <v>0</v>
+      </c>
+      <c r="D15" s="33">
+        <v>1</v>
+      </c>
+      <c r="E15" s="33">
+        <v>0</v>
+      </c>
+      <c r="F15" s="33">
+        <v>0</v>
+      </c>
+      <c r="G15" s="33">
+        <v>1</v>
+      </c>
+      <c r="H15" s="33">
+        <v>0</v>
+      </c>
+      <c r="I15" s="33">
+        <v>0</v>
+      </c>
+      <c r="J15" s="33">
+        <v>40</v>
+      </c>
+      <c r="K15" s="33">
+        <v>50</v>
+      </c>
+      <c r="L15" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="B16" s="33">
+        <v>10</v>
+      </c>
+      <c r="C16" s="33">
+        <v>1</v>
+      </c>
+      <c r="D16" s="33">
+        <v>2</v>
+      </c>
+      <c r="E16" s="33">
+        <v>0</v>
+      </c>
+      <c r="F16" s="33">
+        <v>1</v>
+      </c>
+      <c r="G16" s="33">
+        <v>5</v>
+      </c>
+      <c r="H16" s="33">
+        <v>0</v>
+      </c>
+      <c r="I16" s="33">
+        <v>0</v>
+      </c>
+      <c r="J16" s="33">
+        <v>63</v>
+      </c>
+      <c r="K16" s="33">
+        <v>75</v>
+      </c>
+      <c r="L16" s="33">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>268</v>
+      </c>
+      <c r="B17" s="33">
+        <v>8</v>
+      </c>
+      <c r="C17" s="33">
+        <v>0</v>
+      </c>
+      <c r="D17" s="33">
+        <v>1</v>
+      </c>
+      <c r="E17" s="33">
+        <v>0</v>
+      </c>
+      <c r="F17" s="33">
+        <v>0</v>
+      </c>
+      <c r="G17" s="33">
+        <v>2</v>
+      </c>
+      <c r="H17" s="33">
+        <v>0</v>
+      </c>
+      <c r="I17" s="33">
+        <v>0</v>
+      </c>
+      <c r="J17" s="33">
+        <v>41</v>
+      </c>
+      <c r="K17" s="33">
+        <v>50</v>
+      </c>
+      <c r="L17" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
+        <v>269</v>
+      </c>
+      <c r="B18" s="33">
+        <v>9</v>
+      </c>
+      <c r="C18" s="33">
+        <v>0</v>
+      </c>
+      <c r="D18" s="33">
+        <v>0</v>
+      </c>
+      <c r="E18" s="33">
+        <v>0</v>
+      </c>
+      <c r="F18" s="33">
+        <v>0</v>
+      </c>
+      <c r="G18" s="33">
+        <v>4</v>
+      </c>
+      <c r="H18" s="33">
+        <v>0</v>
+      </c>
+      <c r="I18" s="33">
+        <v>0</v>
+      </c>
+      <c r="J18" s="33">
+        <v>41</v>
+      </c>
+      <c r="K18" s="33">
+        <v>50</v>
+      </c>
+      <c r="L18" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="B19" s="33">
+        <v>1</v>
+      </c>
+      <c r="C19" s="33">
+        <v>0</v>
+      </c>
+      <c r="D19" s="33">
+        <v>1</v>
+      </c>
+      <c r="E19" s="33">
+        <v>0</v>
+      </c>
+      <c r="F19" s="33">
+        <v>0</v>
+      </c>
+      <c r="G19" s="33">
+        <v>7</v>
+      </c>
+      <c r="H19" s="33">
+        <v>0</v>
+      </c>
+      <c r="I19" s="33">
+        <v>0</v>
+      </c>
+      <c r="J19" s="33">
+        <v>48</v>
+      </c>
+      <c r="K19" s="33">
+        <v>50</v>
+      </c>
+      <c r="L19" s="33">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="B20" s="33">
+        <v>7</v>
+      </c>
+      <c r="C20" s="33">
+        <v>1</v>
+      </c>
+      <c r="D20" s="33">
+        <v>0</v>
+      </c>
+      <c r="E20" s="33">
+        <v>0</v>
+      </c>
+      <c r="F20" s="33">
+        <v>1</v>
+      </c>
+      <c r="G20" s="33">
+        <v>4</v>
+      </c>
+      <c r="H20" s="33">
+        <v>0</v>
+      </c>
+      <c r="I20" s="33">
+        <v>0</v>
+      </c>
+      <c r="J20" s="33">
+        <v>37</v>
+      </c>
+      <c r="K20" s="33">
+        <v>44</v>
+      </c>
+      <c r="L20" s="33">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="B21" s="33">
+        <v>11</v>
+      </c>
+      <c r="C21" s="33">
+        <v>0</v>
+      </c>
+      <c r="D21" s="33">
+        <v>0</v>
+      </c>
+      <c r="E21" s="33">
+        <v>0</v>
+      </c>
+      <c r="F21" s="33">
+        <v>0</v>
+      </c>
+      <c r="G21" s="33">
+        <v>4</v>
+      </c>
+      <c r="H21" s="33">
+        <v>0</v>
+      </c>
+      <c r="I21" s="33">
+        <v>0</v>
+      </c>
+      <c r="J21" s="33">
+        <v>39</v>
+      </c>
+      <c r="K21" s="33">
+        <v>50</v>
+      </c>
+      <c r="L21" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="B22" s="33">
+        <v>9</v>
+      </c>
+      <c r="C22" s="33">
+        <v>0</v>
+      </c>
+      <c r="D22" s="33">
+        <v>1</v>
+      </c>
+      <c r="E22" s="33">
+        <v>0</v>
+      </c>
+      <c r="F22" s="33">
+        <v>0</v>
+      </c>
+      <c r="G22" s="33">
+        <v>0</v>
+      </c>
+      <c r="H22" s="33">
+        <v>0</v>
+      </c>
+      <c r="I22" s="33">
+        <v>0</v>
+      </c>
+      <c r="J22" s="33">
+        <v>40</v>
+      </c>
+      <c r="K22" s="33">
+        <v>50</v>
+      </c>
+      <c r="L22" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="B23" s="33">
+        <v>8</v>
+      </c>
+      <c r="C23" s="33">
+        <v>0</v>
+      </c>
+      <c r="D23" s="33">
+        <v>1</v>
+      </c>
+      <c r="E23" s="33">
+        <v>0</v>
+      </c>
+      <c r="F23" s="33">
+        <v>0</v>
+      </c>
+      <c r="G23" s="33">
+        <v>0</v>
+      </c>
+      <c r="H23" s="33">
+        <v>0</v>
+      </c>
+      <c r="I23" s="33">
+        <v>0</v>
+      </c>
+      <c r="J23" s="33">
+        <v>41</v>
+      </c>
+      <c r="K23" s="33">
+        <v>50</v>
+      </c>
+      <c r="L23" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="B24" s="33">
+        <v>4</v>
+      </c>
+      <c r="C24" s="33">
+        <v>0</v>
+      </c>
+      <c r="D24" s="33">
+        <v>0</v>
+      </c>
+      <c r="E24" s="33">
+        <v>0</v>
+      </c>
+      <c r="F24" s="33">
+        <v>0</v>
+      </c>
+      <c r="G24" s="33">
+        <v>0</v>
+      </c>
+      <c r="H24" s="33">
+        <v>0</v>
+      </c>
+      <c r="I24" s="33">
+        <v>0</v>
+      </c>
+      <c r="J24" s="33">
+        <v>46</v>
+      </c>
+      <c r="K24" s="33">
+        <v>50</v>
+      </c>
+      <c r="L24" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="B25" s="33">
+        <v>9</v>
+      </c>
+      <c r="C25" s="33">
+        <v>0</v>
+      </c>
+      <c r="D25" s="33">
+        <v>0</v>
+      </c>
+      <c r="E25" s="33">
+        <v>0</v>
+      </c>
+      <c r="F25" s="33">
+        <v>0</v>
+      </c>
+      <c r="G25" s="33">
+        <v>1</v>
+      </c>
+      <c r="H25" s="33">
+        <v>0</v>
+      </c>
+      <c r="I25" s="33">
+        <v>0</v>
+      </c>
+      <c r="J25" s="33">
+        <v>41</v>
+      </c>
+      <c r="K25" s="33">
+        <v>50</v>
+      </c>
+      <c r="L25" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="B26" s="33">
+        <v>7</v>
+      </c>
+      <c r="C26" s="33">
+        <v>0</v>
+      </c>
+      <c r="D26" s="33">
+        <v>0</v>
+      </c>
+      <c r="E26" s="33">
+        <v>0</v>
+      </c>
+      <c r="F26" s="33">
+        <v>0</v>
+      </c>
+      <c r="G26" s="33">
+        <v>5</v>
+      </c>
+      <c r="H26" s="33">
+        <v>0</v>
+      </c>
+      <c r="I26" s="33">
+        <v>0</v>
+      </c>
+      <c r="J26" s="33">
+        <v>43</v>
+      </c>
+      <c r="K26" s="33">
+        <v>50</v>
+      </c>
+      <c r="L26" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="33" t="s">
+        <v>278</v>
+      </c>
+      <c r="B27" s="33">
+        <v>11</v>
+      </c>
+      <c r="C27" s="33">
+        <v>0</v>
+      </c>
+      <c r="D27" s="33">
+        <v>0</v>
+      </c>
+      <c r="E27" s="33">
+        <v>0</v>
+      </c>
+      <c r="F27" s="33">
+        <v>1</v>
+      </c>
+      <c r="G27" s="33">
+        <v>0</v>
+      </c>
+      <c r="H27" s="33">
+        <v>0</v>
+      </c>
+      <c r="I27" s="33">
+        <v>0</v>
+      </c>
+      <c r="J27" s="33">
+        <v>40</v>
+      </c>
+      <c r="K27" s="33">
+        <v>52</v>
+      </c>
+      <c r="L27" s="33">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
+        <v>279</v>
+      </c>
+      <c r="B28" s="33">
+        <v>8</v>
+      </c>
+      <c r="C28" s="33">
+        <v>0</v>
+      </c>
+      <c r="D28" s="33">
+        <v>0</v>
+      </c>
+      <c r="E28" s="33">
+        <v>0</v>
+      </c>
+      <c r="F28" s="33">
+        <v>0</v>
+      </c>
+      <c r="G28" s="33">
+        <v>3</v>
+      </c>
+      <c r="H28" s="33">
+        <v>0</v>
+      </c>
+      <c r="I28" s="33">
+        <v>0</v>
+      </c>
+      <c r="J28" s="33">
+        <v>42</v>
+      </c>
+      <c r="K28" s="33">
+        <v>50</v>
+      </c>
+      <c r="L28" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="B29" s="33">
+        <v>2</v>
+      </c>
+      <c r="C29" s="33">
+        <v>0</v>
+      </c>
+      <c r="D29" s="33">
+        <v>1</v>
+      </c>
+      <c r="E29" s="33">
+        <v>0</v>
+      </c>
+      <c r="F29" s="33">
+        <v>0</v>
+      </c>
+      <c r="G29" s="33">
+        <v>2</v>
+      </c>
+      <c r="H29" s="33">
+        <v>0</v>
+      </c>
+      <c r="I29" s="33">
+        <v>0</v>
+      </c>
+      <c r="J29" s="33">
+        <v>47</v>
+      </c>
+      <c r="K29" s="33">
+        <v>50</v>
+      </c>
+      <c r="L29" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
+        <v>281</v>
+      </c>
+      <c r="B30" s="33">
+        <v>12</v>
+      </c>
+      <c r="C30" s="33">
+        <v>0</v>
+      </c>
+      <c r="D30" s="33">
+        <v>0</v>
+      </c>
+      <c r="E30" s="33">
+        <v>0</v>
+      </c>
+      <c r="F30" s="33">
+        <v>0</v>
+      </c>
+      <c r="G30" s="33">
+        <v>2</v>
+      </c>
+      <c r="H30" s="33">
+        <v>0</v>
+      </c>
+      <c r="I30" s="33">
+        <v>0</v>
+      </c>
+      <c r="J30" s="33">
+        <v>38</v>
+      </c>
+      <c r="K30" s="33">
+        <v>50</v>
+      </c>
+      <c r="L30" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="B31" s="33">
+        <v>13</v>
+      </c>
+      <c r="C31" s="33">
+        <v>0</v>
+      </c>
+      <c r="D31" s="33">
+        <v>0</v>
+      </c>
+      <c r="E31" s="33">
+        <v>0</v>
+      </c>
+      <c r="F31" s="33">
+        <v>1</v>
+      </c>
+      <c r="G31" s="33">
+        <v>3</v>
+      </c>
+      <c r="H31" s="33">
+        <v>0</v>
+      </c>
+      <c r="I31" s="33">
+        <v>0</v>
+      </c>
+      <c r="J31" s="33">
+        <v>30</v>
+      </c>
+      <c r="K31" s="33">
+        <v>44</v>
+      </c>
+      <c r="L31" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="B32" s="33">
+        <v>4</v>
+      </c>
+      <c r="C32" s="33">
+        <v>0</v>
+      </c>
+      <c r="D32" s="33">
+        <v>0</v>
+      </c>
+      <c r="E32" s="33">
+        <v>0</v>
+      </c>
+      <c r="F32" s="33">
+        <v>0</v>
+      </c>
+      <c r="G32" s="33">
+        <v>3</v>
+      </c>
+      <c r="H32" s="33">
+        <v>0</v>
+      </c>
+      <c r="I32" s="33">
+        <v>0</v>
+      </c>
+      <c r="J32" s="33">
+        <v>46</v>
+      </c>
+      <c r="K32" s="33">
+        <v>50</v>
+      </c>
+      <c r="L32" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
+        <v>284</v>
+      </c>
+      <c r="B33" s="33">
+        <v>5</v>
+      </c>
+      <c r="C33" s="33">
+        <v>0</v>
+      </c>
+      <c r="D33" s="33">
+        <v>0</v>
+      </c>
+      <c r="E33" s="33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="33">
+        <v>0</v>
+      </c>
+      <c r="G33" s="33">
+        <v>2</v>
+      </c>
+      <c r="H33" s="33">
+        <v>0</v>
+      </c>
+      <c r="I33" s="33">
+        <v>0</v>
+      </c>
+      <c r="J33" s="33">
+        <v>45</v>
+      </c>
+      <c r="K33" s="33">
+        <v>50</v>
+      </c>
+      <c r="L33" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="33" t="s">
+        <v>285</v>
+      </c>
+      <c r="B34" s="33">
+        <v>12</v>
+      </c>
+      <c r="C34" s="33">
+        <v>0</v>
+      </c>
+      <c r="D34" s="33">
+        <v>0</v>
+      </c>
+      <c r="E34" s="33">
+        <v>0</v>
+      </c>
+      <c r="F34" s="33">
+        <v>1</v>
+      </c>
+      <c r="G34" s="33">
+        <v>0</v>
+      </c>
+      <c r="H34" s="33">
+        <v>0</v>
+      </c>
+      <c r="I34" s="33">
+        <v>0</v>
+      </c>
+      <c r="J34" s="33">
+        <v>65</v>
+      </c>
+      <c r="K34" s="33">
+        <v>78</v>
+      </c>
+      <c r="L34" s="33">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="33" t="s">
+        <v>286</v>
+      </c>
+      <c r="B35" s="33">
+        <v>1</v>
+      </c>
+      <c r="C35" s="33">
+        <v>0</v>
+      </c>
+      <c r="D35" s="33">
+        <v>0</v>
+      </c>
+      <c r="E35" s="33">
+        <v>0</v>
+      </c>
+      <c r="F35" s="33">
+        <v>0</v>
+      </c>
+      <c r="G35" s="33">
+        <v>1</v>
+      </c>
+      <c r="H35" s="33">
+        <v>0</v>
+      </c>
+      <c r="I35" s="33">
+        <v>0</v>
+      </c>
+      <c r="J35" s="33">
+        <v>49</v>
+      </c>
+      <c r="K35" s="33">
+        <v>50</v>
+      </c>
+      <c r="L35" s="33">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="B36" s="33">
+        <v>5</v>
+      </c>
+      <c r="C36" s="33">
+        <v>0</v>
+      </c>
+      <c r="D36" s="33">
+        <v>0</v>
+      </c>
+      <c r="E36" s="33">
+        <v>0</v>
+      </c>
+      <c r="F36" s="33">
+        <v>0</v>
+      </c>
+      <c r="G36" s="33">
+        <v>2</v>
+      </c>
+      <c r="H36" s="33">
+        <v>0</v>
+      </c>
+      <c r="I36" s="33">
+        <v>0</v>
+      </c>
+      <c r="J36" s="33">
+        <v>45</v>
+      </c>
+      <c r="K36" s="33">
+        <v>50</v>
+      </c>
+      <c r="L36" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="s">
+        <v>288</v>
+      </c>
+      <c r="B37" s="33">
+        <v>10</v>
+      </c>
+      <c r="C37" s="33">
+        <v>1</v>
+      </c>
+      <c r="D37" s="33">
+        <v>0</v>
+      </c>
+      <c r="E37" s="33">
+        <v>0</v>
+      </c>
+      <c r="F37" s="33">
+        <v>1</v>
+      </c>
+      <c r="G37" s="33">
+        <v>2</v>
+      </c>
+      <c r="H37" s="33">
+        <v>0</v>
+      </c>
+      <c r="I37" s="33">
+        <v>0</v>
+      </c>
+      <c r="J37" s="33">
+        <v>62</v>
+      </c>
+      <c r="K37" s="33">
+        <v>72</v>
+      </c>
+      <c r="L37" s="33">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
+        <v>289</v>
+      </c>
+      <c r="B38" s="33">
+        <v>2</v>
+      </c>
+      <c r="C38" s="33">
+        <v>0</v>
+      </c>
+      <c r="D38" s="33">
+        <v>0</v>
+      </c>
+      <c r="E38" s="33">
+        <v>0</v>
+      </c>
+      <c r="F38" s="33">
+        <v>0</v>
+      </c>
+      <c r="G38" s="33">
+        <v>3</v>
+      </c>
+      <c r="H38" s="33">
+        <v>0</v>
+      </c>
+      <c r="I38" s="33">
+        <v>0</v>
+      </c>
+      <c r="J38" s="33">
+        <v>48</v>
+      </c>
+      <c r="K38" s="33">
+        <v>50</v>
+      </c>
+      <c r="L38" s="33">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="33" t="s">
+        <v>290</v>
+      </c>
+      <c r="B39" s="33">
+        <v>7</v>
+      </c>
+      <c r="C39" s="33">
+        <v>0</v>
+      </c>
+      <c r="D39" s="33">
+        <v>0</v>
+      </c>
+      <c r="E39" s="33">
+        <v>0</v>
+      </c>
+      <c r="F39" s="33">
+        <v>0</v>
+      </c>
+      <c r="G39" s="33">
+        <v>2</v>
+      </c>
+      <c r="H39" s="33">
+        <v>0</v>
+      </c>
+      <c r="I39" s="33">
+        <v>0</v>
+      </c>
+      <c r="J39" s="33">
+        <v>43</v>
+      </c>
+      <c r="K39" s="33">
+        <v>50</v>
+      </c>
+      <c r="L39" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
+        <v>291</v>
+      </c>
+      <c r="B40" s="33">
+        <v>16</v>
+      </c>
+      <c r="C40" s="33">
+        <v>0</v>
+      </c>
+      <c r="D40" s="33">
+        <v>0</v>
+      </c>
+      <c r="E40" s="33">
+        <v>0</v>
+      </c>
+      <c r="F40" s="33">
+        <v>0</v>
+      </c>
+      <c r="G40" s="33">
+        <v>0</v>
+      </c>
+      <c r="H40" s="33">
+        <v>0</v>
+      </c>
+      <c r="I40" s="33">
+        <v>0</v>
+      </c>
+      <c r="J40" s="33">
+        <v>34</v>
+      </c>
+      <c r="K40" s="33">
+        <v>50</v>
+      </c>
+      <c r="L40" s="33">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="33" t="s">
+        <v>292</v>
+      </c>
+      <c r="B41" s="33">
+        <v>12</v>
+      </c>
+      <c r="C41" s="33">
+        <v>0</v>
+      </c>
+      <c r="D41" s="33">
+        <v>0</v>
+      </c>
+      <c r="E41" s="33">
+        <v>0</v>
+      </c>
+      <c r="F41" s="33">
+        <v>0</v>
+      </c>
+      <c r="G41" s="33">
+        <v>2</v>
+      </c>
+      <c r="H41" s="33">
+        <v>0</v>
+      </c>
+      <c r="I41" s="33">
+        <v>0</v>
+      </c>
+      <c r="J41" s="33">
+        <v>38</v>
+      </c>
+      <c r="K41" s="33">
+        <v>50</v>
+      </c>
+      <c r="L41" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
+        <v>293</v>
+      </c>
+      <c r="B42" s="33">
+        <v>7</v>
+      </c>
+      <c r="C42" s="33">
+        <v>1</v>
+      </c>
+      <c r="D42" s="33">
+        <v>0</v>
+      </c>
+      <c r="E42" s="33">
+        <v>0</v>
+      </c>
+      <c r="F42" s="33">
+        <v>1</v>
+      </c>
+      <c r="G42" s="33">
+        <v>4</v>
+      </c>
+      <c r="H42" s="33">
+        <v>0</v>
+      </c>
+      <c r="I42" s="33">
+        <v>0</v>
+      </c>
+      <c r="J42" s="33">
+        <v>39</v>
+      </c>
+      <c r="K42" s="33">
+        <v>46</v>
+      </c>
+      <c r="L42" s="33">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="s">
+        <v>294</v>
+      </c>
+      <c r="B43" s="33">
+        <v>8</v>
+      </c>
+      <c r="C43" s="33">
+        <v>0</v>
+      </c>
+      <c r="D43" s="33">
+        <v>1</v>
+      </c>
+      <c r="E43" s="33">
+        <v>0</v>
+      </c>
+      <c r="F43" s="33">
+        <v>0</v>
+      </c>
+      <c r="G43" s="33">
+        <v>4</v>
+      </c>
+      <c r="H43" s="33">
+        <v>0</v>
+      </c>
+      <c r="I43" s="33">
+        <v>0</v>
+      </c>
+      <c r="J43" s="33">
+        <v>41</v>
+      </c>
+      <c r="K43" s="33">
+        <v>50</v>
+      </c>
+      <c r="L43" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="s">
+        <v>295</v>
+      </c>
+      <c r="B44" s="33">
+        <v>6</v>
+      </c>
+      <c r="C44" s="33">
+        <v>0</v>
+      </c>
+      <c r="D44" s="33">
+        <v>0</v>
+      </c>
+      <c r="E44" s="33">
+        <v>0</v>
+      </c>
+      <c r="F44" s="33">
+        <v>0</v>
+      </c>
+      <c r="G44" s="33">
+        <v>2</v>
+      </c>
+      <c r="H44" s="33">
+        <v>0</v>
+      </c>
+      <c r="I44" s="33">
+        <v>0</v>
+      </c>
+      <c r="J44" s="33">
+        <v>45</v>
+      </c>
+      <c r="K44" s="33">
+        <v>50</v>
+      </c>
+      <c r="L44" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="s">
+        <v>296</v>
+      </c>
+      <c r="B45" s="33">
+        <v>6</v>
+      </c>
+      <c r="C45" s="33">
+        <v>0</v>
+      </c>
+      <c r="D45" s="33">
+        <v>5</v>
+      </c>
+      <c r="E45" s="33">
+        <v>0</v>
+      </c>
+      <c r="F45" s="33">
+        <v>0</v>
+      </c>
+      <c r="G45" s="33">
+        <v>2</v>
+      </c>
+      <c r="H45" s="33">
+        <v>0</v>
+      </c>
+      <c r="I45" s="33">
+        <v>0</v>
+      </c>
+      <c r="J45" s="33">
+        <v>39</v>
+      </c>
+      <c r="K45" s="33">
+        <v>50</v>
+      </c>
+      <c r="L45" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
+        <v>297</v>
+      </c>
+      <c r="B46" s="33">
+        <v>9</v>
+      </c>
+      <c r="C46" s="33">
+        <v>0</v>
+      </c>
+      <c r="D46" s="33">
+        <v>0</v>
+      </c>
+      <c r="E46" s="33">
+        <v>0</v>
+      </c>
+      <c r="F46" s="33">
+        <v>0</v>
+      </c>
+      <c r="G46" s="33">
+        <v>6</v>
+      </c>
+      <c r="H46" s="33">
+        <v>0</v>
+      </c>
+      <c r="I46" s="33">
+        <v>0</v>
+      </c>
+      <c r="J46" s="33">
+        <v>41</v>
+      </c>
+      <c r="K46" s="33">
+        <v>50</v>
+      </c>
+      <c r="L46" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="33" t="s">
+        <v>298</v>
+      </c>
+      <c r="B47" s="33">
+        <v>10</v>
+      </c>
+      <c r="C47" s="33">
+        <v>0</v>
+      </c>
+      <c r="D47" s="33">
+        <v>0</v>
+      </c>
+      <c r="E47" s="33">
+        <v>0</v>
+      </c>
+      <c r="F47" s="33">
+        <v>0</v>
+      </c>
+      <c r="G47" s="33">
+        <v>4</v>
+      </c>
+      <c r="H47" s="33">
+        <v>0</v>
+      </c>
+      <c r="I47" s="33">
+        <v>0</v>
+      </c>
+      <c r="J47" s="33">
+        <v>40</v>
+      </c>
+      <c r="K47" s="33">
+        <v>50</v>
+      </c>
+      <c r="L47" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="B48" s="33">
+        <v>7</v>
+      </c>
+      <c r="C48" s="33">
+        <v>0</v>
+      </c>
+      <c r="D48" s="33">
+        <v>0</v>
+      </c>
+      <c r="E48" s="33">
+        <v>0</v>
+      </c>
+      <c r="F48" s="33">
+        <v>1</v>
+      </c>
+      <c r="G48" s="33">
+        <v>2</v>
+      </c>
+      <c r="H48" s="33">
+        <v>0</v>
+      </c>
+      <c r="I48" s="33">
+        <v>0</v>
+      </c>
+      <c r="J48" s="33">
+        <v>29</v>
+      </c>
+      <c r="K48" s="33">
+        <v>37</v>
+      </c>
+      <c r="L48" s="33">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="B49" s="33">
+        <v>4</v>
+      </c>
+      <c r="C49" s="33">
+        <v>0</v>
+      </c>
+      <c r="D49" s="33">
+        <v>0</v>
+      </c>
+      <c r="E49" s="33">
+        <v>0</v>
+      </c>
+      <c r="F49" s="33">
+        <v>0</v>
+      </c>
+      <c r="G49" s="33">
+        <v>3</v>
+      </c>
+      <c r="H49" s="33">
+        <v>0</v>
+      </c>
+      <c r="I49" s="33">
+        <v>0</v>
+      </c>
+      <c r="J49" s="33">
+        <v>46</v>
+      </c>
+      <c r="K49" s="33">
+        <v>50</v>
+      </c>
+      <c r="L49" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="s">
+        <v>301</v>
+      </c>
+      <c r="B50" s="33">
+        <v>3</v>
+      </c>
+      <c r="C50" s="33">
+        <v>0</v>
+      </c>
+      <c r="D50" s="33">
+        <v>0</v>
+      </c>
+      <c r="E50" s="33">
+        <v>0</v>
+      </c>
+      <c r="F50" s="33">
+        <v>0</v>
+      </c>
+      <c r="G50" s="33">
+        <v>3</v>
+      </c>
+      <c r="H50" s="33">
+        <v>0</v>
+      </c>
+      <c r="I50" s="33">
+        <v>0</v>
+      </c>
+      <c r="J50" s="33">
+        <v>47</v>
+      </c>
+      <c r="K50" s="33">
+        <v>50</v>
+      </c>
+      <c r="L50" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="33" t="s">
+        <v>302</v>
+      </c>
+      <c r="B51" s="33">
+        <v>6</v>
+      </c>
+      <c r="C51" s="33">
+        <v>0</v>
+      </c>
+      <c r="D51" s="33">
+        <v>0</v>
+      </c>
+      <c r="E51" s="33">
+        <v>0</v>
+      </c>
+      <c r="F51" s="33">
+        <v>0</v>
+      </c>
+      <c r="G51" s="33">
+        <v>3</v>
+      </c>
+      <c r="H51" s="33">
+        <v>0</v>
+      </c>
+      <c r="I51" s="33">
+        <v>0</v>
+      </c>
+      <c r="J51" s="33">
+        <v>44</v>
+      </c>
+      <c r="K51" s="33">
+        <v>50</v>
+      </c>
+      <c r="L51" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
+        <v>303</v>
+      </c>
+      <c r="B52" s="33">
+        <v>5</v>
+      </c>
+      <c r="C52" s="33">
+        <v>0</v>
+      </c>
+      <c r="D52" s="33">
+        <v>0</v>
+      </c>
+      <c r="E52" s="33">
+        <v>0</v>
+      </c>
+      <c r="F52" s="33">
+        <v>1</v>
+      </c>
+      <c r="G52" s="33">
+        <v>9</v>
+      </c>
+      <c r="H52" s="33">
+        <v>0</v>
+      </c>
+      <c r="I52" s="33">
+        <v>0</v>
+      </c>
+      <c r="J52" s="33">
+        <v>64</v>
+      </c>
+      <c r="K52" s="33">
+        <v>70</v>
+      </c>
+      <c r="L52" s="33">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="34" t="s">
+        <v>304</v>
+      </c>
+      <c r="B53" s="34">
+        <f>SUM(B2:B52)</f>
+        <v>398</v>
+      </c>
+      <c r="C53" s="34">
+        <f t="shared" ref="C53:L53" si="0">SUM(C2:C52)</f>
+        <v>5</v>
+      </c>
+      <c r="D53" s="34">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E53" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="34">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G53" s="34">
+        <f t="shared" si="0"/>
+        <v>149</v>
+      </c>
+      <c r="H53" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I53" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J53" s="34">
+        <f t="shared" si="0"/>
+        <v>2206</v>
+      </c>
+      <c r="K53" s="34">
+        <f t="shared" si="0"/>
+        <v>2626</v>
+      </c>
+      <c r="L53" s="34">
+        <f t="shared" si="0"/>
+        <v>3036</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="38"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="37"/>
+      <c r="E54" t="s">
+        <v>39</v>
+      </c>
+      <c r="F54">
+        <f>G53</f>
+        <v>149</v>
+      </c>
+      <c r="J54">
+        <f>B53-C53</f>
+        <v>393</v>
+      </c>
+      <c r="K54" s="37"/>
+      <c r="L54" s="37"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>40</v>
+      </c>
+      <c r="F55">
+        <f>B53</f>
+        <v>398</v>
+      </c>
+      <c r="J55">
+        <f>D53-E53</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>41</v>
+      </c>
+      <c r="F56">
+        <v>12</v>
+      </c>
+      <c r="J56">
+        <f>F62</f>
+        <v>2626</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>42</v>
+      </c>
+      <c r="F57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F58" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="J58" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <f>SUM(F54:F58)</f>
+        <v>564</v>
+      </c>
+      <c r="J59">
+        <f>SUM(J54:J58)</f>
+        <v>3036</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>45</v>
+      </c>
+      <c r="F60">
+        <f>K53-F59</f>
+        <v>2062</v>
+      </c>
+      <c r="J60" s="35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F61" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="J61">
+        <f>J59-L53</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <f>F60+F59</f>
+        <v>2626</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <f>F62-K53</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:K31"/>
   <sheetViews>

</xml_diff>

<commit_message>
nmv 13 01 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 6.1 TO 6.6.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 6.1 TO 6.6.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02AD10D-1A12-4E3D-BD58-77129137A504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777FA517-E17D-4592-A0FC-329439F1F48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="6.1" sheetId="15" r:id="rId1"/>
     <sheet name="6.2" sheetId="16" r:id="rId2"/>
     <sheet name="6.3" sheetId="17" r:id="rId3"/>
     <sheet name="6.4" sheetId="18" r:id="rId4"/>
-    <sheet name="total 6.1 to 6.6" sheetId="7" r:id="rId5"/>
+    <sheet name="6.5" sheetId="19" r:id="rId5"/>
+    <sheet name="total 6.1 to 6.6" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="348">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -2149,6 +2150,135 @@
   </si>
   <si>
     <t>51</t>
+  </si>
+  <si>
+    <t>6.5.1.1 :</t>
+  </si>
+  <si>
+    <t>6.5.1.2 :</t>
+  </si>
+  <si>
+    <t>6.5.1.3 :</t>
+  </si>
+  <si>
+    <t>6.5.1.4 :</t>
+  </si>
+  <si>
+    <t>6.5.1.5 :</t>
+  </si>
+  <si>
+    <t>6.5.2.1 :</t>
+  </si>
+  <si>
+    <t>6.5.2.2 :</t>
+  </si>
+  <si>
+    <t>6.5.2.3 :</t>
+  </si>
+  <si>
+    <t>6.5.3.1 :</t>
+  </si>
+  <si>
+    <t>6.5.3.2 :</t>
+  </si>
+  <si>
+    <t>6.5.3.3 :</t>
+  </si>
+  <si>
+    <t>6.5.3.4 :</t>
+  </si>
+  <si>
+    <t>6.5.4.1 :</t>
+  </si>
+  <si>
+    <t>6.5.4.2 :</t>
+  </si>
+  <si>
+    <t>6.5.5.1 :</t>
+  </si>
+  <si>
+    <t>6.5.5.2 :</t>
+  </si>
+  <si>
+    <t>6.5.5.3 :</t>
+  </si>
+  <si>
+    <t>6.5.6.1 :</t>
+  </si>
+  <si>
+    <t>6.5.6.2 :</t>
+  </si>
+  <si>
+    <t>6.5.6.3 :</t>
+  </si>
+  <si>
+    <t>6.5.6.4 :</t>
+  </si>
+  <si>
+    <t>6.5.6.5 :</t>
+  </si>
+  <si>
+    <t>6.5.7.1 :</t>
+  </si>
+  <si>
+    <t>6.5.7.2 :</t>
+  </si>
+  <si>
+    <t>6.5.7.3 :</t>
+  </si>
+  <si>
+    <t>6.5.8.1 :</t>
+  </si>
+  <si>
+    <t>6.5.8.2 :</t>
+  </si>
+  <si>
+    <t>6.5.8.3 :</t>
+  </si>
+  <si>
+    <t>6.5.8.4 :</t>
+  </si>
+  <si>
+    <t>6.5.8.5 :</t>
+  </si>
+  <si>
+    <t>6.5.8.6 :</t>
+  </si>
+  <si>
+    <t>6.5.9.1 :</t>
+  </si>
+  <si>
+    <t>6.5.9.2 :</t>
+  </si>
+  <si>
+    <t>6.5.9.3 :</t>
+  </si>
+  <si>
+    <t>6.5.9.4 :</t>
+  </si>
+  <si>
+    <t>6.5.10.1 :</t>
+  </si>
+  <si>
+    <t>6.5.10.2 :</t>
+  </si>
+  <si>
+    <t>6.5.10.3 :</t>
+  </si>
+  <si>
+    <t>6.5.11.1 :</t>
+  </si>
+  <si>
+    <t>6.5.11.2 :</t>
+  </si>
+  <si>
+    <t>6.5.11.3 :</t>
+  </si>
+  <si>
+    <t>6.5.11.4 :</t>
+  </si>
+  <si>
+    <t>42</t>
   </si>
 </sst>
 </file>
@@ -2443,8 +2573,8 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -10853,9 +10983,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95756750-C929-4133-9B35-850FD96AC5E9}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L44" sqref="L44"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13006,6 +13136,1816 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A3F2C4-245C-4DDC-AE07-B168A8A6AD4C}">
+  <dimension ref="A1:L54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:L44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>305</v>
+      </c>
+      <c r="B2" s="33">
+        <v>1</v>
+      </c>
+      <c r="C2" s="33">
+        <v>0</v>
+      </c>
+      <c r="D2" s="33">
+        <v>0</v>
+      </c>
+      <c r="E2" s="33">
+        <v>0</v>
+      </c>
+      <c r="F2" s="33">
+        <v>0</v>
+      </c>
+      <c r="G2" s="33">
+        <v>7</v>
+      </c>
+      <c r="H2" s="33">
+        <v>0</v>
+      </c>
+      <c r="I2" s="33">
+        <v>0</v>
+      </c>
+      <c r="J2" s="33">
+        <v>49</v>
+      </c>
+      <c r="K2" s="33">
+        <v>50</v>
+      </c>
+      <c r="L2" s="33">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>306</v>
+      </c>
+      <c r="B3" s="33">
+        <v>1</v>
+      </c>
+      <c r="C3" s="33">
+        <v>0</v>
+      </c>
+      <c r="D3" s="33">
+        <v>0</v>
+      </c>
+      <c r="E3" s="33">
+        <v>0</v>
+      </c>
+      <c r="F3" s="33">
+        <v>0</v>
+      </c>
+      <c r="G3" s="33">
+        <v>6</v>
+      </c>
+      <c r="H3" s="33">
+        <v>0</v>
+      </c>
+      <c r="I3" s="33">
+        <v>0</v>
+      </c>
+      <c r="J3" s="33">
+        <v>49</v>
+      </c>
+      <c r="K3" s="33">
+        <v>50</v>
+      </c>
+      <c r="L3" s="33">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="B4" s="33">
+        <v>5</v>
+      </c>
+      <c r="C4" s="33">
+        <v>0</v>
+      </c>
+      <c r="D4" s="33">
+        <v>0</v>
+      </c>
+      <c r="E4" s="33">
+        <v>0</v>
+      </c>
+      <c r="F4" s="33">
+        <v>0</v>
+      </c>
+      <c r="G4" s="33">
+        <v>3</v>
+      </c>
+      <c r="H4" s="33">
+        <v>0</v>
+      </c>
+      <c r="I4" s="33">
+        <v>0</v>
+      </c>
+      <c r="J4" s="33">
+        <v>45</v>
+      </c>
+      <c r="K4" s="33">
+        <v>50</v>
+      </c>
+      <c r="L4" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>308</v>
+      </c>
+      <c r="B5" s="33">
+        <v>5</v>
+      </c>
+      <c r="C5" s="33">
+        <v>0</v>
+      </c>
+      <c r="D5" s="33">
+        <v>0</v>
+      </c>
+      <c r="E5" s="33">
+        <v>0</v>
+      </c>
+      <c r="F5" s="33">
+        <v>0</v>
+      </c>
+      <c r="G5" s="33">
+        <v>3</v>
+      </c>
+      <c r="H5" s="33">
+        <v>0</v>
+      </c>
+      <c r="I5" s="33">
+        <v>0</v>
+      </c>
+      <c r="J5" s="33">
+        <v>45</v>
+      </c>
+      <c r="K5" s="33">
+        <v>50</v>
+      </c>
+      <c r="L5" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>309</v>
+      </c>
+      <c r="B6" s="33">
+        <v>6</v>
+      </c>
+      <c r="C6" s="33">
+        <v>0</v>
+      </c>
+      <c r="D6" s="33">
+        <v>1</v>
+      </c>
+      <c r="E6" s="33">
+        <v>0</v>
+      </c>
+      <c r="F6" s="33">
+        <v>1</v>
+      </c>
+      <c r="G6" s="33">
+        <v>2</v>
+      </c>
+      <c r="H6" s="33">
+        <v>0</v>
+      </c>
+      <c r="I6" s="33">
+        <v>0</v>
+      </c>
+      <c r="J6" s="33">
+        <v>25</v>
+      </c>
+      <c r="K6" s="33">
+        <v>33</v>
+      </c>
+      <c r="L6" s="33">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="B7" s="33">
+        <v>5</v>
+      </c>
+      <c r="C7" s="33">
+        <v>0</v>
+      </c>
+      <c r="D7" s="33">
+        <v>0</v>
+      </c>
+      <c r="E7" s="33">
+        <v>0</v>
+      </c>
+      <c r="F7" s="33">
+        <v>0</v>
+      </c>
+      <c r="G7" s="33">
+        <v>0</v>
+      </c>
+      <c r="H7" s="33">
+        <v>0</v>
+      </c>
+      <c r="I7" s="33">
+        <v>0</v>
+      </c>
+      <c r="J7" s="33">
+        <v>45</v>
+      </c>
+      <c r="K7" s="33">
+        <v>50</v>
+      </c>
+      <c r="L7" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="B8" s="33">
+        <v>12</v>
+      </c>
+      <c r="C8" s="33">
+        <v>0</v>
+      </c>
+      <c r="D8" s="33">
+        <v>0</v>
+      </c>
+      <c r="E8" s="33">
+        <v>0</v>
+      </c>
+      <c r="F8" s="33">
+        <v>0</v>
+      </c>
+      <c r="G8" s="33">
+        <v>0</v>
+      </c>
+      <c r="H8" s="33">
+        <v>0</v>
+      </c>
+      <c r="I8" s="33">
+        <v>0</v>
+      </c>
+      <c r="J8" s="33">
+        <v>38</v>
+      </c>
+      <c r="K8" s="33">
+        <v>50</v>
+      </c>
+      <c r="L8" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="B9" s="33">
+        <v>9</v>
+      </c>
+      <c r="C9" s="33">
+        <v>0</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0</v>
+      </c>
+      <c r="E9" s="33">
+        <v>0</v>
+      </c>
+      <c r="F9" s="33">
+        <v>1</v>
+      </c>
+      <c r="G9" s="33">
+        <v>1</v>
+      </c>
+      <c r="H9" s="33">
+        <v>0</v>
+      </c>
+      <c r="I9" s="33">
+        <v>0</v>
+      </c>
+      <c r="J9" s="33">
+        <v>29</v>
+      </c>
+      <c r="K9" s="33">
+        <v>39</v>
+      </c>
+      <c r="L9" s="33">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="B10" s="33">
+        <v>15</v>
+      </c>
+      <c r="C10" s="33">
+        <v>0</v>
+      </c>
+      <c r="D10" s="33">
+        <v>2</v>
+      </c>
+      <c r="E10" s="33">
+        <v>0</v>
+      </c>
+      <c r="F10" s="33">
+        <v>0</v>
+      </c>
+      <c r="G10" s="33">
+        <v>2</v>
+      </c>
+      <c r="H10" s="33">
+        <v>0</v>
+      </c>
+      <c r="I10" s="33">
+        <v>0</v>
+      </c>
+      <c r="J10" s="33">
+        <v>33</v>
+      </c>
+      <c r="K10" s="33">
+        <v>50</v>
+      </c>
+      <c r="L10" s="33">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>314</v>
+      </c>
+      <c r="B11" s="33">
+        <v>5</v>
+      </c>
+      <c r="C11" s="33">
+        <v>0</v>
+      </c>
+      <c r="D11" s="33">
+        <v>0</v>
+      </c>
+      <c r="E11" s="33">
+        <v>0</v>
+      </c>
+      <c r="F11" s="33">
+        <v>0</v>
+      </c>
+      <c r="G11" s="33">
+        <v>3</v>
+      </c>
+      <c r="H11" s="33">
+        <v>0</v>
+      </c>
+      <c r="I11" s="33">
+        <v>0</v>
+      </c>
+      <c r="J11" s="33">
+        <v>45</v>
+      </c>
+      <c r="K11" s="33">
+        <v>50</v>
+      </c>
+      <c r="L11" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="B12" s="33">
+        <v>7</v>
+      </c>
+      <c r="C12" s="33">
+        <v>0</v>
+      </c>
+      <c r="D12" s="33">
+        <v>0</v>
+      </c>
+      <c r="E12" s="33">
+        <v>0</v>
+      </c>
+      <c r="F12" s="33">
+        <v>0</v>
+      </c>
+      <c r="G12" s="33">
+        <v>6</v>
+      </c>
+      <c r="H12" s="33">
+        <v>0</v>
+      </c>
+      <c r="I12" s="33">
+        <v>0</v>
+      </c>
+      <c r="J12" s="33">
+        <v>43</v>
+      </c>
+      <c r="K12" s="33">
+        <v>50</v>
+      </c>
+      <c r="L12" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="B13" s="33">
+        <v>9</v>
+      </c>
+      <c r="C13" s="33">
+        <v>0</v>
+      </c>
+      <c r="D13" s="33">
+        <v>0</v>
+      </c>
+      <c r="E13" s="33">
+        <v>0</v>
+      </c>
+      <c r="F13" s="33">
+        <v>1</v>
+      </c>
+      <c r="G13" s="33">
+        <v>1</v>
+      </c>
+      <c r="H13" s="33">
+        <v>0</v>
+      </c>
+      <c r="I13" s="33">
+        <v>0</v>
+      </c>
+      <c r="J13" s="33">
+        <v>24</v>
+      </c>
+      <c r="K13" s="33">
+        <v>34</v>
+      </c>
+      <c r="L13" s="33">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="B14" s="33">
+        <v>14</v>
+      </c>
+      <c r="C14" s="33">
+        <v>0</v>
+      </c>
+      <c r="D14" s="33">
+        <v>2</v>
+      </c>
+      <c r="E14" s="33">
+        <v>0</v>
+      </c>
+      <c r="F14" s="33">
+        <v>0</v>
+      </c>
+      <c r="G14" s="33">
+        <v>1</v>
+      </c>
+      <c r="H14" s="33">
+        <v>0</v>
+      </c>
+      <c r="I14" s="33">
+        <v>0</v>
+      </c>
+      <c r="J14" s="33">
+        <v>34</v>
+      </c>
+      <c r="K14" s="33">
+        <v>50</v>
+      </c>
+      <c r="L14" s="33">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="B15" s="33">
+        <v>8</v>
+      </c>
+      <c r="C15" s="33">
+        <v>0</v>
+      </c>
+      <c r="D15" s="33">
+        <v>0</v>
+      </c>
+      <c r="E15" s="33">
+        <v>0</v>
+      </c>
+      <c r="F15" s="33">
+        <v>1</v>
+      </c>
+      <c r="G15" s="33">
+        <v>3</v>
+      </c>
+      <c r="H15" s="33">
+        <v>0</v>
+      </c>
+      <c r="I15" s="33">
+        <v>0</v>
+      </c>
+      <c r="J15" s="33">
+        <v>21</v>
+      </c>
+      <c r="K15" s="33">
+        <v>30</v>
+      </c>
+      <c r="L15" s="33">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>319</v>
+      </c>
+      <c r="B16" s="33">
+        <v>6</v>
+      </c>
+      <c r="C16" s="33">
+        <v>0</v>
+      </c>
+      <c r="D16" s="33">
+        <v>0</v>
+      </c>
+      <c r="E16" s="33">
+        <v>0</v>
+      </c>
+      <c r="F16" s="33">
+        <v>0</v>
+      </c>
+      <c r="G16" s="33">
+        <v>3</v>
+      </c>
+      <c r="H16" s="33">
+        <v>0</v>
+      </c>
+      <c r="I16" s="33">
+        <v>0</v>
+      </c>
+      <c r="J16" s="33">
+        <v>44</v>
+      </c>
+      <c r="K16" s="33">
+        <v>50</v>
+      </c>
+      <c r="L16" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>320</v>
+      </c>
+      <c r="B17" s="33">
+        <v>2</v>
+      </c>
+      <c r="C17" s="33">
+        <v>0</v>
+      </c>
+      <c r="D17" s="33">
+        <v>0</v>
+      </c>
+      <c r="E17" s="33">
+        <v>0</v>
+      </c>
+      <c r="F17" s="33">
+        <v>0</v>
+      </c>
+      <c r="G17" s="33">
+        <v>5</v>
+      </c>
+      <c r="H17" s="33">
+        <v>0</v>
+      </c>
+      <c r="I17" s="33">
+        <v>0</v>
+      </c>
+      <c r="J17" s="33">
+        <v>48</v>
+      </c>
+      <c r="K17" s="33">
+        <v>50</v>
+      </c>
+      <c r="L17" s="33">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
+        <v>321</v>
+      </c>
+      <c r="B18" s="33">
+        <v>17</v>
+      </c>
+      <c r="C18" s="33">
+        <v>0</v>
+      </c>
+      <c r="D18" s="33">
+        <v>0</v>
+      </c>
+      <c r="E18" s="33">
+        <v>0</v>
+      </c>
+      <c r="F18" s="33">
+        <v>1</v>
+      </c>
+      <c r="G18" s="33">
+        <v>4</v>
+      </c>
+      <c r="H18" s="33">
+        <v>0</v>
+      </c>
+      <c r="I18" s="33">
+        <v>0</v>
+      </c>
+      <c r="J18" s="33">
+        <v>60</v>
+      </c>
+      <c r="K18" s="33">
+        <v>78</v>
+      </c>
+      <c r="L18" s="33">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
+        <v>322</v>
+      </c>
+      <c r="B19" s="33">
+        <v>6</v>
+      </c>
+      <c r="C19" s="33">
+        <v>0</v>
+      </c>
+      <c r="D19" s="33">
+        <v>0</v>
+      </c>
+      <c r="E19" s="33">
+        <v>0</v>
+      </c>
+      <c r="F19" s="33">
+        <v>0</v>
+      </c>
+      <c r="G19" s="33">
+        <v>2</v>
+      </c>
+      <c r="H19" s="33">
+        <v>0</v>
+      </c>
+      <c r="I19" s="33">
+        <v>0</v>
+      </c>
+      <c r="J19" s="33">
+        <v>44</v>
+      </c>
+      <c r="K19" s="33">
+        <v>50</v>
+      </c>
+      <c r="L19" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>323</v>
+      </c>
+      <c r="B20" s="33">
+        <v>2</v>
+      </c>
+      <c r="C20" s="33">
+        <v>0</v>
+      </c>
+      <c r="D20" s="33">
+        <v>0</v>
+      </c>
+      <c r="E20" s="33">
+        <v>0</v>
+      </c>
+      <c r="F20" s="33">
+        <v>0</v>
+      </c>
+      <c r="G20" s="33">
+        <v>0</v>
+      </c>
+      <c r="H20" s="33">
+        <v>0</v>
+      </c>
+      <c r="I20" s="33">
+        <v>0</v>
+      </c>
+      <c r="J20" s="33">
+        <v>48</v>
+      </c>
+      <c r="K20" s="33">
+        <v>50</v>
+      </c>
+      <c r="L20" s="33">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
+        <v>324</v>
+      </c>
+      <c r="B21" s="33">
+        <v>8</v>
+      </c>
+      <c r="C21" s="33">
+        <v>0</v>
+      </c>
+      <c r="D21" s="33">
+        <v>0</v>
+      </c>
+      <c r="E21" s="33">
+        <v>0</v>
+      </c>
+      <c r="F21" s="33">
+        <v>0</v>
+      </c>
+      <c r="G21" s="33">
+        <v>7</v>
+      </c>
+      <c r="H21" s="33">
+        <v>0</v>
+      </c>
+      <c r="I21" s="33">
+        <v>0</v>
+      </c>
+      <c r="J21" s="33">
+        <v>42</v>
+      </c>
+      <c r="K21" s="33">
+        <v>50</v>
+      </c>
+      <c r="L21" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
+        <v>325</v>
+      </c>
+      <c r="B22" s="33">
+        <v>5</v>
+      </c>
+      <c r="C22" s="33">
+        <v>0</v>
+      </c>
+      <c r="D22" s="33">
+        <v>0</v>
+      </c>
+      <c r="E22" s="33">
+        <v>0</v>
+      </c>
+      <c r="F22" s="33">
+        <v>0</v>
+      </c>
+      <c r="G22" s="33">
+        <v>0</v>
+      </c>
+      <c r="H22" s="33">
+        <v>0</v>
+      </c>
+      <c r="I22" s="33">
+        <v>0</v>
+      </c>
+      <c r="J22" s="33">
+        <v>45</v>
+      </c>
+      <c r="K22" s="33">
+        <v>50</v>
+      </c>
+      <c r="L22" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="B23" s="33">
+        <v>15</v>
+      </c>
+      <c r="C23" s="33">
+        <v>1</v>
+      </c>
+      <c r="D23" s="33">
+        <v>0</v>
+      </c>
+      <c r="E23" s="33">
+        <v>0</v>
+      </c>
+      <c r="F23" s="33">
+        <v>1</v>
+      </c>
+      <c r="G23" s="33">
+        <v>6</v>
+      </c>
+      <c r="H23" s="33">
+        <v>0</v>
+      </c>
+      <c r="I23" s="33">
+        <v>0</v>
+      </c>
+      <c r="J23" s="33">
+        <v>62</v>
+      </c>
+      <c r="K23" s="33">
+        <v>77</v>
+      </c>
+      <c r="L23" s="33">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>327</v>
+      </c>
+      <c r="B24" s="33">
+        <v>10</v>
+      </c>
+      <c r="C24" s="33">
+        <v>0</v>
+      </c>
+      <c r="D24" s="33">
+        <v>0</v>
+      </c>
+      <c r="E24" s="33">
+        <v>0</v>
+      </c>
+      <c r="F24" s="33">
+        <v>0</v>
+      </c>
+      <c r="G24" s="33">
+        <v>2</v>
+      </c>
+      <c r="H24" s="33">
+        <v>0</v>
+      </c>
+      <c r="I24" s="33">
+        <v>0</v>
+      </c>
+      <c r="J24" s="33">
+        <v>40</v>
+      </c>
+      <c r="K24" s="33">
+        <v>50</v>
+      </c>
+      <c r="L24" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
+        <v>328</v>
+      </c>
+      <c r="B25" s="33">
+        <v>14</v>
+      </c>
+      <c r="C25" s="33">
+        <v>0</v>
+      </c>
+      <c r="D25" s="33">
+        <v>0</v>
+      </c>
+      <c r="E25" s="33">
+        <v>0</v>
+      </c>
+      <c r="F25" s="33">
+        <v>0</v>
+      </c>
+      <c r="G25" s="33">
+        <v>5</v>
+      </c>
+      <c r="H25" s="33">
+        <v>0</v>
+      </c>
+      <c r="I25" s="33">
+        <v>0</v>
+      </c>
+      <c r="J25" s="33">
+        <v>36</v>
+      </c>
+      <c r="K25" s="33">
+        <v>50</v>
+      </c>
+      <c r="L25" s="33">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="33" t="s">
+        <v>329</v>
+      </c>
+      <c r="B26" s="33">
+        <v>9</v>
+      </c>
+      <c r="C26" s="33">
+        <v>0</v>
+      </c>
+      <c r="D26" s="33">
+        <v>0</v>
+      </c>
+      <c r="E26" s="33">
+        <v>0</v>
+      </c>
+      <c r="F26" s="33">
+        <v>1</v>
+      </c>
+      <c r="G26" s="33">
+        <v>2</v>
+      </c>
+      <c r="H26" s="33">
+        <v>0</v>
+      </c>
+      <c r="I26" s="33">
+        <v>0</v>
+      </c>
+      <c r="J26" s="33">
+        <v>59</v>
+      </c>
+      <c r="K26" s="33">
+        <v>69</v>
+      </c>
+      <c r="L26" s="33">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="33" t="s">
+        <v>330</v>
+      </c>
+      <c r="B27" s="33">
+        <v>19</v>
+      </c>
+      <c r="C27" s="33">
+        <v>0</v>
+      </c>
+      <c r="D27" s="33">
+        <v>1</v>
+      </c>
+      <c r="E27" s="33">
+        <v>0</v>
+      </c>
+      <c r="F27" s="33">
+        <v>0</v>
+      </c>
+      <c r="G27" s="33">
+        <v>6</v>
+      </c>
+      <c r="H27" s="33">
+        <v>0</v>
+      </c>
+      <c r="I27" s="33">
+        <v>0</v>
+      </c>
+      <c r="J27" s="33">
+        <v>30</v>
+      </c>
+      <c r="K27" s="33">
+        <v>50</v>
+      </c>
+      <c r="L27" s="33">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
+        <v>331</v>
+      </c>
+      <c r="B28" s="33">
+        <v>10</v>
+      </c>
+      <c r="C28" s="33">
+        <v>0</v>
+      </c>
+      <c r="D28" s="33">
+        <v>0</v>
+      </c>
+      <c r="E28" s="33">
+        <v>0</v>
+      </c>
+      <c r="F28" s="33">
+        <v>0</v>
+      </c>
+      <c r="G28" s="33">
+        <v>3</v>
+      </c>
+      <c r="H28" s="33">
+        <v>0</v>
+      </c>
+      <c r="I28" s="33">
+        <v>0</v>
+      </c>
+      <c r="J28" s="33">
+        <v>40</v>
+      </c>
+      <c r="K28" s="33">
+        <v>50</v>
+      </c>
+      <c r="L28" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="s">
+        <v>332</v>
+      </c>
+      <c r="B29" s="33">
+        <v>7</v>
+      </c>
+      <c r="C29" s="33">
+        <v>0</v>
+      </c>
+      <c r="D29" s="33">
+        <v>1</v>
+      </c>
+      <c r="E29" s="33">
+        <v>0</v>
+      </c>
+      <c r="F29" s="33">
+        <v>0</v>
+      </c>
+      <c r="G29" s="33">
+        <v>3</v>
+      </c>
+      <c r="H29" s="33">
+        <v>0</v>
+      </c>
+      <c r="I29" s="33">
+        <v>0</v>
+      </c>
+      <c r="J29" s="33">
+        <v>42</v>
+      </c>
+      <c r="K29" s="33">
+        <v>50</v>
+      </c>
+      <c r="L29" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
+        <v>333</v>
+      </c>
+      <c r="B30" s="33">
+        <v>7</v>
+      </c>
+      <c r="C30" s="33">
+        <v>0</v>
+      </c>
+      <c r="D30" s="33">
+        <v>0</v>
+      </c>
+      <c r="E30" s="33">
+        <v>0</v>
+      </c>
+      <c r="F30" s="33">
+        <v>0</v>
+      </c>
+      <c r="G30" s="33">
+        <v>5</v>
+      </c>
+      <c r="H30" s="33">
+        <v>0</v>
+      </c>
+      <c r="I30" s="33">
+        <v>0</v>
+      </c>
+      <c r="J30" s="33">
+        <v>43</v>
+      </c>
+      <c r="K30" s="33">
+        <v>50</v>
+      </c>
+      <c r="L30" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
+        <v>334</v>
+      </c>
+      <c r="B31" s="33">
+        <v>15</v>
+      </c>
+      <c r="C31" s="33">
+        <v>0</v>
+      </c>
+      <c r="D31" s="33">
+        <v>0</v>
+      </c>
+      <c r="E31" s="33">
+        <v>0</v>
+      </c>
+      <c r="F31" s="33">
+        <v>0</v>
+      </c>
+      <c r="G31" s="33">
+        <v>6</v>
+      </c>
+      <c r="H31" s="33">
+        <v>0</v>
+      </c>
+      <c r="I31" s="33">
+        <v>0</v>
+      </c>
+      <c r="J31" s="33">
+        <v>35</v>
+      </c>
+      <c r="K31" s="33">
+        <v>50</v>
+      </c>
+      <c r="L31" s="33">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="s">
+        <v>335</v>
+      </c>
+      <c r="B32" s="33">
+        <v>9</v>
+      </c>
+      <c r="C32" s="33">
+        <v>0</v>
+      </c>
+      <c r="D32" s="33">
+        <v>0</v>
+      </c>
+      <c r="E32" s="33">
+        <v>0</v>
+      </c>
+      <c r="F32" s="33">
+        <v>1</v>
+      </c>
+      <c r="G32" s="33">
+        <v>8</v>
+      </c>
+      <c r="H32" s="33">
+        <v>0</v>
+      </c>
+      <c r="I32" s="33">
+        <v>0</v>
+      </c>
+      <c r="J32" s="33">
+        <v>48</v>
+      </c>
+      <c r="K32" s="33">
+        <v>58</v>
+      </c>
+      <c r="L32" s="33">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
+        <v>336</v>
+      </c>
+      <c r="B33" s="33">
+        <v>4</v>
+      </c>
+      <c r="C33" s="33">
+        <v>0</v>
+      </c>
+      <c r="D33" s="33">
+        <v>0</v>
+      </c>
+      <c r="E33" s="33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="33">
+        <v>0</v>
+      </c>
+      <c r="G33" s="33">
+        <v>3</v>
+      </c>
+      <c r="H33" s="33">
+        <v>0</v>
+      </c>
+      <c r="I33" s="33">
+        <v>0</v>
+      </c>
+      <c r="J33" s="33">
+        <v>46</v>
+      </c>
+      <c r="K33" s="33">
+        <v>50</v>
+      </c>
+      <c r="L33" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="33" t="s">
+        <v>337</v>
+      </c>
+      <c r="B34" s="33">
+        <v>11</v>
+      </c>
+      <c r="C34" s="33">
+        <v>0</v>
+      </c>
+      <c r="D34" s="33">
+        <v>3</v>
+      </c>
+      <c r="E34" s="33">
+        <v>0</v>
+      </c>
+      <c r="F34" s="33">
+        <v>0</v>
+      </c>
+      <c r="G34" s="33">
+        <v>0</v>
+      </c>
+      <c r="H34" s="33">
+        <v>0</v>
+      </c>
+      <c r="I34" s="33">
+        <v>0</v>
+      </c>
+      <c r="J34" s="33">
+        <v>36</v>
+      </c>
+      <c r="K34" s="33">
+        <v>50</v>
+      </c>
+      <c r="L34" s="33">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="33" t="s">
+        <v>338</v>
+      </c>
+      <c r="B35" s="33">
+        <v>14</v>
+      </c>
+      <c r="C35" s="33">
+        <v>0</v>
+      </c>
+      <c r="D35" s="33">
+        <v>0</v>
+      </c>
+      <c r="E35" s="33">
+        <v>0</v>
+      </c>
+      <c r="F35" s="33">
+        <v>0</v>
+      </c>
+      <c r="G35" s="33">
+        <v>2</v>
+      </c>
+      <c r="H35" s="33">
+        <v>0</v>
+      </c>
+      <c r="I35" s="33">
+        <v>0</v>
+      </c>
+      <c r="J35" s="33">
+        <v>36</v>
+      </c>
+      <c r="K35" s="33">
+        <v>50</v>
+      </c>
+      <c r="L35" s="33">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="33" t="s">
+        <v>339</v>
+      </c>
+      <c r="B36" s="33">
+        <v>7</v>
+      </c>
+      <c r="C36" s="33">
+        <v>0</v>
+      </c>
+      <c r="D36" s="33">
+        <v>0</v>
+      </c>
+      <c r="E36" s="33">
+        <v>0</v>
+      </c>
+      <c r="F36" s="33">
+        <v>1</v>
+      </c>
+      <c r="G36" s="33">
+        <v>7</v>
+      </c>
+      <c r="H36" s="33">
+        <v>0</v>
+      </c>
+      <c r="I36" s="33">
+        <v>0</v>
+      </c>
+      <c r="J36" s="33">
+        <v>42</v>
+      </c>
+      <c r="K36" s="33">
+        <v>50</v>
+      </c>
+      <c r="L36" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="s">
+        <v>340</v>
+      </c>
+      <c r="B37" s="33">
+        <v>12</v>
+      </c>
+      <c r="C37" s="33">
+        <v>0</v>
+      </c>
+      <c r="D37" s="33">
+        <v>0</v>
+      </c>
+      <c r="E37" s="33">
+        <v>0</v>
+      </c>
+      <c r="F37" s="33">
+        <v>0</v>
+      </c>
+      <c r="G37" s="33">
+        <v>2</v>
+      </c>
+      <c r="H37" s="33">
+        <v>0</v>
+      </c>
+      <c r="I37" s="33">
+        <v>0</v>
+      </c>
+      <c r="J37" s="33">
+        <v>38</v>
+      </c>
+      <c r="K37" s="33">
+        <v>50</v>
+      </c>
+      <c r="L37" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
+        <v>341</v>
+      </c>
+      <c r="B38" s="33">
+        <v>5</v>
+      </c>
+      <c r="C38" s="33">
+        <v>0</v>
+      </c>
+      <c r="D38" s="33">
+        <v>0</v>
+      </c>
+      <c r="E38" s="33">
+        <v>0</v>
+      </c>
+      <c r="F38" s="33">
+        <v>0</v>
+      </c>
+      <c r="G38" s="33">
+        <v>2</v>
+      </c>
+      <c r="H38" s="33">
+        <v>0</v>
+      </c>
+      <c r="I38" s="33">
+        <v>0</v>
+      </c>
+      <c r="J38" s="33">
+        <v>45</v>
+      </c>
+      <c r="K38" s="33">
+        <v>50</v>
+      </c>
+      <c r="L38" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="33" t="s">
+        <v>342</v>
+      </c>
+      <c r="B39" s="33">
+        <v>10</v>
+      </c>
+      <c r="C39" s="33">
+        <v>0</v>
+      </c>
+      <c r="D39" s="33">
+        <v>0</v>
+      </c>
+      <c r="E39" s="33">
+        <v>0</v>
+      </c>
+      <c r="F39" s="33">
+        <v>1</v>
+      </c>
+      <c r="G39" s="33">
+        <v>6</v>
+      </c>
+      <c r="H39" s="33">
+        <v>0</v>
+      </c>
+      <c r="I39" s="33">
+        <v>0</v>
+      </c>
+      <c r="J39" s="33">
+        <v>57</v>
+      </c>
+      <c r="K39" s="33">
+        <v>68</v>
+      </c>
+      <c r="L39" s="33">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
+        <v>343</v>
+      </c>
+      <c r="B40" s="33">
+        <v>4</v>
+      </c>
+      <c r="C40" s="33">
+        <v>0</v>
+      </c>
+      <c r="D40" s="33">
+        <v>0</v>
+      </c>
+      <c r="E40" s="33">
+        <v>0</v>
+      </c>
+      <c r="F40" s="33">
+        <v>0</v>
+      </c>
+      <c r="G40" s="33">
+        <v>6</v>
+      </c>
+      <c r="H40" s="33">
+        <v>0</v>
+      </c>
+      <c r="I40" s="33">
+        <v>0</v>
+      </c>
+      <c r="J40" s="33">
+        <v>46</v>
+      </c>
+      <c r="K40" s="33">
+        <v>50</v>
+      </c>
+      <c r="L40" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="33" t="s">
+        <v>344</v>
+      </c>
+      <c r="B41" s="33">
+        <v>8</v>
+      </c>
+      <c r="C41" s="33">
+        <v>0</v>
+      </c>
+      <c r="D41" s="33">
+        <v>0</v>
+      </c>
+      <c r="E41" s="33">
+        <v>0</v>
+      </c>
+      <c r="F41" s="33">
+        <v>0</v>
+      </c>
+      <c r="G41" s="33">
+        <v>6</v>
+      </c>
+      <c r="H41" s="33">
+        <v>0</v>
+      </c>
+      <c r="I41" s="33">
+        <v>0</v>
+      </c>
+      <c r="J41" s="33">
+        <v>42</v>
+      </c>
+      <c r="K41" s="33">
+        <v>50</v>
+      </c>
+      <c r="L41" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
+        <v>345</v>
+      </c>
+      <c r="B42" s="33">
+        <v>8</v>
+      </c>
+      <c r="C42" s="33">
+        <v>0</v>
+      </c>
+      <c r="D42" s="33">
+        <v>0</v>
+      </c>
+      <c r="E42" s="33">
+        <v>0</v>
+      </c>
+      <c r="F42" s="33">
+        <v>0</v>
+      </c>
+      <c r="G42" s="33">
+        <v>2</v>
+      </c>
+      <c r="H42" s="33">
+        <v>0</v>
+      </c>
+      <c r="I42" s="33">
+        <v>0</v>
+      </c>
+      <c r="J42" s="33">
+        <v>42</v>
+      </c>
+      <c r="K42" s="33">
+        <v>50</v>
+      </c>
+      <c r="L42" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="s">
+        <v>346</v>
+      </c>
+      <c r="B43" s="33">
+        <v>10</v>
+      </c>
+      <c r="C43" s="33">
+        <v>1</v>
+      </c>
+      <c r="D43" s="33">
+        <v>0</v>
+      </c>
+      <c r="E43" s="33">
+        <v>0</v>
+      </c>
+      <c r="F43" s="33">
+        <v>1</v>
+      </c>
+      <c r="G43" s="33">
+        <v>5</v>
+      </c>
+      <c r="H43" s="33">
+        <v>0</v>
+      </c>
+      <c r="I43" s="33">
+        <v>0</v>
+      </c>
+      <c r="J43" s="33">
+        <v>54</v>
+      </c>
+      <c r="K43" s="33">
+        <v>64</v>
+      </c>
+      <c r="L43" s="33">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="B44" s="36">
+        <f>SUM(B2:B43)</f>
+        <v>356</v>
+      </c>
+      <c r="C44" s="36">
+        <f t="shared" ref="C44:L44" si="0">SUM(C2:C43)</f>
+        <v>2</v>
+      </c>
+      <c r="D44" s="36">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E44" s="36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F44" s="36">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G44" s="36">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="H44" s="36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I44" s="36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J44" s="36">
+        <f t="shared" si="0"/>
+        <v>1775</v>
+      </c>
+      <c r="K44" s="36">
+        <f t="shared" si="0"/>
+        <v>2150</v>
+      </c>
+      <c r="L44" s="36">
+        <f t="shared" si="0"/>
+        <v>2514</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="32"/>
+      <c r="D45" s="37"/>
+      <c r="E45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F45">
+        <f>G44</f>
+        <v>146</v>
+      </c>
+      <c r="J45">
+        <f>B44-C44</f>
+        <v>354</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>40</v>
+      </c>
+      <c r="F46">
+        <f>B44</f>
+        <v>356</v>
+      </c>
+      <c r="J46">
+        <f>D44-E44</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47">
+        <v>6</v>
+      </c>
+      <c r="J47">
+        <f>F53</f>
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>42</v>
+      </c>
+      <c r="F48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F49" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="J49" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <f>SUM(F45:F49)</f>
+        <v>512</v>
+      </c>
+      <c r="J50">
+        <f>SUM(J45:J49)</f>
+        <v>2514</v>
+      </c>
+    </row>
+    <row r="51" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>45</v>
+      </c>
+      <c r="F51">
+        <f>K44-F50</f>
+        <v>1638</v>
+      </c>
+      <c r="J51" s="35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F52" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="J52">
+        <f>J50-L44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <f>F51+F50</f>
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="54" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <f>F53-K44</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:K31"/>
   <sheetViews>

</xml_diff>